<commit_message>
1. Make process result return two dictionaries 2. Update the burndown chart
</commit_message>
<xml_diff>
--- a/TeamGZWReport.xlsx
+++ b/TeamGZWReport.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\SIT\SSW555\SSW555Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaojieli/Desktop/Spring2018/SSW555/Project/SSW555Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005" tabRatio="993" activeTab="4"/>
+    <workbookView xWindow="4220" yWindow="2100" windowWidth="25600" windowHeight="15560" tabRatio="993" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Sprint4" sheetId="8" r:id="rId8"/>
     <sheet name="Stories" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="220">
   <si>
     <t>Initials</t>
   </si>
@@ -705,46 +705,22 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>19+21+</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>45+40+</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>Actual Remaining Stories</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Planned Remaining Stories</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>N/A</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>N/A</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>N/A</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>N/A</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="176" formatCode="m/d"/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
-    <numFmt numFmtId="178" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="164" formatCode="m/d"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -835,13 +811,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -851,22 +827,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -950,9 +926,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:style val="18"/>
   <c:chart>
@@ -998,7 +974,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1011,19 +987,19 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41065</c:v>
+                  <c:v>41065.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41078</c:v>
+                  <c:v>41078.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41092</c:v>
+                  <c:v>41092.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41106</c:v>
+                  <c:v>41106.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41120</c:v>
+                  <c:v>41120.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1035,25 +1011,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F690-4477-BD90-CBFE7542BB78}"/>
             </c:ext>
@@ -1076,11 +1052,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1414572864"/>
-        <c:axId val="-1415743968"/>
+        <c:axId val="82372096"/>
+        <c:axId val="82390736"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-1414572864"/>
+        <c:axId val="82372096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1115,17 +1091,17 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1415743968"/>
+        <c:crossAx val="82390736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-1415743968"/>
+        <c:axId val="82390736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1170,10 +1146,10 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1414572864"/>
+        <c:crossAx val="82372096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1207,262 +1183,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <c:style val="18"/>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="4A7EBB"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="4A7EBB"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>Burndown!$A$2:$A$7</c:f>
-              <c:numCache>
-                <c:formatCode>m/d</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>41681</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41688</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41695</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41702</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41709</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41716</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Burndown!$C$2:$C$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5615-40BC-A87E-8CB856C1E36C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="-1414961632"/>
-        <c:axId val="-1414959312"/>
-      </c:lineChart>
-      <c:dateAx>
-        <c:axId val="-1414961632"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="878787"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-1414959312"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="0"/>
-        <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-        <c:majorUnit val="1"/>
-        <c:majorTimeUnit val="days"/>
-      </c:dateAx>
-      <c:valAx>
-        <c:axId val="-1414959312"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="878787"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-1414961632"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="25400">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1474,6 +1197,40 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Burndown</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:t>Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1499,7 +1256,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1546,22 +1303,10 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41681</c:v>
+                  <c:v>41681.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41688</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41695</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41702</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41709</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41716</c:v>
+                  <c:v>41695.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1573,28 +1318,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-65F3-44CB-887C-3143EE86AB37}"/>
             </c:ext>
@@ -1637,22 +1370,10 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41681</c:v>
+                  <c:v>41681.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41688</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41695</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41702</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41709</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41716</c:v>
+                  <c:v>41695.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1664,28 +1385,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-65F3-44CB-887C-3143EE86AB37}"/>
             </c:ext>
@@ -1701,11 +1410,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1172165791"/>
-        <c:axId val="1099778719"/>
+        <c:axId val="81934384"/>
+        <c:axId val="81935744"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="1172165791"/>
+        <c:axId val="81934384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1745,17 +1454,17 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1099778719"/>
+        <c:crossAx val="81935744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="1099778719"/>
+        <c:axId val="81935744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1803,10 +1512,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1172165791"/>
+        <c:crossAx val="81934384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1844,7 +1553,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2418,7 +2127,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2454,7 +2163,7 @@
         <xdr:cNvPr id="3" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2576,7 +2285,7 @@
         <xdr:cNvPr id="4" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2671,7 +2380,7 @@
         <xdr:cNvPr id="5" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2766,7 +2475,7 @@
         <xdr:cNvPr id="6" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2888,7 +2597,7 @@
         <xdr:cNvPr id="7" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2983,7 +2692,7 @@
         <xdr:cNvPr id="8" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3065,25 +2774,25 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>81720</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>160920</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>418042</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>70909</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>340290</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
+      <xdr:colOff>754593</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>3175</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 1">
+        <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3096,42 +2805,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3175</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>644525</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>130175</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="图表 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3409,12 +3082,12 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="15.625" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3431,7 +3104,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -3448,7 +3121,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3465,7 +3138,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -3482,7 +3155,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="D9" s="1" t="s">
         <v>19</v>
       </c>
@@ -3490,13 +3163,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E10" s="15" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="E10" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3521,12 +3194,12 @@
       <selection activeCell="E3" sqref="B3:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -3546,7 +3219,7 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3567,7 +3240,7 @@
       <c r="AMI2"/>
       <c r="AMJ2"/>
     </row>
-    <row r="3" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3588,24 +3261,24 @@
       <c r="AMI3"/>
       <c r="AMJ3"/>
     </row>
-    <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3622,7 +3295,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3639,24 +3312,24 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="17" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>2</v>
       </c>
@@ -3670,7 +3343,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>2</v>
       </c>
@@ -3684,7 +3357,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>2</v>
       </c>
@@ -3698,7 +3371,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2</v>
       </c>
@@ -3712,7 +3385,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2</v>
       </c>
@@ -3726,7 +3399,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2</v>
       </c>
@@ -3740,7 +3413,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>3</v>
       </c>
@@ -3754,7 +3427,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>3</v>
       </c>
@@ -3768,7 +3441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>3</v>
       </c>
@@ -3782,7 +3455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>3</v>
       </c>
@@ -3796,7 +3469,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>3</v>
       </c>
@@ -3810,7 +3483,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>3</v>
       </c>
@@ -3824,7 +3497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>4</v>
       </c>
@@ -3838,7 +3511,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>4</v>
       </c>
@@ -3852,7 +3525,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>4</v>
       </c>
@@ -3866,7 +3539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>4</v>
       </c>
@@ -3880,7 +3553,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>4</v>
       </c>
@@ -3894,7 +3567,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>4</v>
       </c>
@@ -3923,49 +3596,49 @@
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="3"/>
-    <col min="6" max="6" width="8.875" style="4"/>
+    <col min="1" max="1" width="8.83203125" style="3"/>
+    <col min="6" max="6" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>76</v>
       </c>
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>77</v>
       </c>
       <c r="F2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>78</v>
       </c>
       <c r="F3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>79</v>
       </c>
       <c r="F5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>80</v>
       </c>
       <c r="F6"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>81</v>
       </c>
       <c r="F8"/>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -3988,7 +3661,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>88</v>
       </c>
@@ -4004,7 +3677,7 @@
       <c r="F15" s="8"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>89</v>
       </c>
@@ -4029,7 +3702,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
         <v>90</v>
       </c>
@@ -4054,7 +3727,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
         <v>91</v>
       </c>
@@ -4079,7 +3752,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
         <v>92</v>
       </c>
@@ -4116,28 +3789,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="18.625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="22.375" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="6" max="6" width="19.75" customWidth="1"/>
-    <col min="7" max="7" width="8.875" style="4"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>82</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>84</v>
@@ -4152,7 +3827,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>41681</v>
       </c>
@@ -4167,9 +3842,9 @@
       </c>
       <c r="G2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
-        <v>41688</v>
+        <v>41695</v>
       </c>
       <c r="B3">
         <v>18</v>
@@ -4181,116 +3856,30 @@
         <f>C2-C3</f>
         <v>6</v>
       </c>
-      <c r="E3" t="s">
-        <v>218</v>
-      </c>
-      <c r="F3" t="s">
-        <v>219</v>
-      </c>
-      <c r="G3" s="4" t="e">
+      <c r="E3">
+        <f>19+21+10+12+24+29</f>
+        <v>115</v>
+      </c>
+      <c r="F3">
+        <f>45+40+25+30+40+30</f>
+        <v>210</v>
+      </c>
+      <c r="G3" s="4">
         <f>(E3-E2)/F3*60</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>41695</v>
-      </c>
-      <c r="B4">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>222</v>
-      </c>
-      <c r="D4" t="e">
-        <f>C3-C4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E4" t="s">
-        <v>222</v>
-      </c>
-      <c r="F4" t="s">
-        <v>223</v>
-      </c>
-      <c r="G4" s="4" t="e">
-        <f>(E4-E3)/F4*60</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>41702</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>222</v>
-      </c>
-      <c r="D5" t="e">
-        <f>C4-C5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E5" t="s">
-        <v>222</v>
-      </c>
-      <c r="F5" t="s">
-        <v>225</v>
-      </c>
-      <c r="G5" s="4" t="e">
-        <f>(E5-E4)/F5*60</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>41709</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>223</v>
-      </c>
-      <c r="D6" t="e">
-        <f>C5-C6</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E6" t="s">
-        <v>224</v>
-      </c>
-      <c r="F6" t="s">
-        <v>222</v>
-      </c>
-      <c r="G6" s="4" t="e">
-        <f>(E6-E5)/F6*60</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>41716</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>223</v>
-      </c>
-      <c r="D7" t="e">
-        <f>C6-C7</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E7" t="s">
-        <v>223</v>
-      </c>
-      <c r="F7" t="s">
-        <v>223</v>
-      </c>
-      <c r="G7" s="4" t="e">
-        <f>(E7-E6)/F7*60</f>
-        <v>#VALUE!</v>
-      </c>
+        <v>32.857142857142861</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -4304,21 +3893,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="26.125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="15.125" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="17.625" customWidth="1"/>
-    <col min="8" max="8" width="17.875" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" customWidth="1"/>
     <col min="9" max="9" width="13.5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -4347,12 +3936,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="I2" s="5">
         <v>41679</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -4377,11 +3966,11 @@
       <c r="H3" s="1">
         <v>45</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>96</v>
       </c>
@@ -4393,7 +3982,7 @@
       </c>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>98</v>
       </c>
@@ -4405,7 +3994,7 @@
       </c>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -4417,7 +4006,7 @@
       </c>
       <c r="I6"/>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
@@ -4442,11 +4031,11 @@
       <c r="H7" s="1">
         <v>40</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>102</v>
       </c>
@@ -4458,7 +4047,7 @@
       </c>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>104</v>
       </c>
@@ -4470,7 +4059,7 @@
       </c>
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -4482,11 +4071,11 @@
       </c>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B11"/>
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
@@ -4512,7 +4101,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>192</v>
       </c>
@@ -4538,7 +4127,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>195</v>
       </c>
@@ -4564,7 +4153,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>197</v>
       </c>
@@ -4590,7 +4179,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
@@ -4617,7 +4206,7 @@
       </c>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>199</v>
       </c>
@@ -4643,7 +4232,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>201</v>
       </c>
@@ -4669,7 +4258,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>203</v>
       </c>
@@ -4695,7 +4284,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>48</v>
       </c>
@@ -4706,17 +4295,23 @@
         <v>15</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>29</v>
+        <v>194</v>
       </c>
       <c r="E22" s="1">
         <v>30</v>
       </c>
       <c r="F22" s="1">
-        <v>2</v>
+        <v>40</v>
+      </c>
+      <c r="G22" s="1">
+        <v>24</v>
+      </c>
+      <c r="H22" s="1">
+        <v>40</v>
       </c>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>206</v>
       </c>
@@ -4724,7 +4319,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>208</v>
       </c>
@@ -4732,7 +4327,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>52</v>
       </c>
@@ -4743,17 +4338,23 @@
         <v>15</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>29</v>
+        <v>194</v>
       </c>
       <c r="E26" s="1">
         <v>30</v>
       </c>
       <c r="F26" s="1">
-        <v>2</v>
+        <v>40</v>
+      </c>
+      <c r="G26" s="1">
+        <v>29</v>
+      </c>
+      <c r="H26" s="1">
+        <v>30</v>
       </c>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>210</v>
       </c>
@@ -4761,7 +4362,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="39" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>212</v>
       </c>
@@ -4784,9 +4385,9 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -4830,9 +4431,9 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -4876,9 +4477,9 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -4922,13 +4523,13 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="251.875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="251.83203125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -4939,7 +4540,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -4950,7 +4551,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -4961,7 +4562,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -4972,7 +4573,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -4983,7 +4584,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -4994,7 +4595,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -5005,7 +4606,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -5016,7 +4617,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -5027,7 +4628,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -5038,7 +4639,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -5049,7 +4650,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>123</v>
       </c>
@@ -5060,7 +4661,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>126</v>
       </c>
@@ -5071,7 +4672,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -5082,7 +4683,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>130</v>
       </c>
@@ -5093,7 +4694,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>133</v>
       </c>
@@ -5104,7 +4705,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -5115,7 +4716,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -5126,7 +4727,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>68</v>
       </c>
@@ -5137,7 +4738,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>139</v>
       </c>
@@ -5148,7 +4749,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>142</v>
       </c>
@@ -5159,7 +4760,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>145</v>
       </c>
@@ -5170,7 +4771,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>148</v>
       </c>
@@ -5181,7 +4782,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>151</v>
       </c>
@@ -5192,7 +4793,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>154</v>
       </c>
@@ -5203,7 +4804,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>157</v>
       </c>
@@ -5214,7 +4815,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -5225,7 +4826,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -5236,7 +4837,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -5247,7 +4848,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -5258,7 +4859,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -5269,7 +4870,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -5280,7 +4881,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>168</v>
       </c>
@@ -5291,7 +4892,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>171</v>
       </c>
@@ -5302,7 +4903,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>174</v>
       </c>
@@ -5313,7 +4914,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>177</v>
       </c>
@@ -5324,7 +4925,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>180</v>
       </c>
@@ -5335,7 +4936,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>183</v>
       </c>
@@ -5346,7 +4947,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>64</v>
       </c>
@@ -5357,7 +4958,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>70</v>
       </c>
@@ -5368,7 +4969,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>27</v>
       </c>
@@ -5379,7 +4980,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -5390,7 +4991,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Update with user stories from GL and acceptance test
</commit_message>
<xml_diff>
--- a/TeamGZWReport.xlsx
+++ b/TeamGZWReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4220" yWindow="2100" windowWidth="25600" windowHeight="15560" tabRatio="993" activeTab="3"/>
+    <workbookView xWindow="12840" yWindow="0" windowWidth="12760" windowHeight="16000" tabRatio="993" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="219">
   <si>
     <t>Initials</t>
   </si>
@@ -660,9 +660,6 @@
   <si>
     <t>Compare marriage date to birth date</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Birth before mariage</t>
   </si>
   <si>
     <t>T02.01</t>
@@ -1052,11 +1049,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="82372096"/>
-        <c:axId val="82390736"/>
+        <c:axId val="-777706736"/>
+        <c:axId val="-777704416"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="82372096"/>
+        <c:axId val="-777706736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1094,14 +1091,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82390736"/>
+        <c:crossAx val="-777704416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="82390736"/>
+        <c:axId val="-777704416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1149,7 +1146,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82372096"/>
+        <c:crossAx val="-777706736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1410,11 +1407,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="81934384"/>
-        <c:axId val="81935744"/>
+        <c:axId val="-773490928"/>
+        <c:axId val="-773488880"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="81934384"/>
+        <c:axId val="-773490928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1457,14 +1454,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81935744"/>
+        <c:crossAx val="-773488880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="81935744"/>
+        <c:axId val="-773488880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1515,7 +1512,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81934384"/>
+        <c:crossAx val="-773490928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2127,7 +2124,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2163,7 +2160,7 @@
         <xdr:cNvPr id="3" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2285,7 +2282,7 @@
         <xdr:cNvPr id="4" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2380,7 +2377,7 @@
         <xdr:cNvPr id="5" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2475,7 +2472,7 @@
         <xdr:cNvPr id="6" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2597,7 +2594,7 @@
         <xdr:cNvPr id="7" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2692,7 +2689,7 @@
         <xdr:cNvPr id="8" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2792,7 +2789,7 @@
         <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3275,7 +3272,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:1024" x14ac:dyDescent="0.15">
@@ -3326,7 +3323,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:1024" x14ac:dyDescent="0.15">
@@ -3789,7 +3786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -3809,10 +3806,10 @@
         <v>82</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>84</v>
@@ -3893,8 +3890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3924,13 +3921,13 @@
         <v>93</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>94</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>95</v>
@@ -3952,7 +3949,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E3" s="1">
         <v>50</v>
@@ -4017,7 +4014,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E7" s="1">
         <v>80</v>
@@ -4289,7 +4286,7 @@
         <v>48</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>205</v>
+        <v>49</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>15</v>
@@ -4313,18 +4310,18 @@
     </row>
     <row r="23" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
+        <v>205</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>206</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
+        <v>207</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>208</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
@@ -4356,18 +4353,18 @@
     </row>
     <row r="27" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
+        <v>209</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>210</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="39" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
+        <v>211</v>
+      </c>
+      <c r="B28" s="10" t="s">
         <v>212</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -4520,7 +4517,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4826,7 +4823,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Minor updates in Product Backlog
</commit_message>
<xml_diff>
--- a/TeamGZWReport.xlsx
+++ b/TeamGZWReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12840" yWindow="0" windowWidth="12760" windowHeight="16000" tabRatio="993" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" tabRatio="993" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -1049,11 +1049,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-777706736"/>
-        <c:axId val="-777704416"/>
+        <c:axId val="-749505984"/>
+        <c:axId val="-736218096"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-777706736"/>
+        <c:axId val="-749505984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1091,14 +1091,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-777704416"/>
+        <c:crossAx val="-736218096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-777704416"/>
+        <c:axId val="-736218096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1146,7 +1146,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-777706736"/>
+        <c:crossAx val="-749505984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1227,7 +1227,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1407,11 +1406,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-773490928"/>
-        <c:axId val="-773488880"/>
+        <c:axId val="-736203104"/>
+        <c:axId val="-736201056"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-773490928"/>
+        <c:axId val="-736203104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1454,14 +1453,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773488880"/>
+        <c:crossAx val="-736201056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-773488880"/>
+        <c:axId val="-736201056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1512,7 +1511,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773490928"/>
+        <c:crossAx val="-736203104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2124,7 +2123,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2160,7 +2159,7 @@
         <xdr:cNvPr id="3" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2282,7 +2281,7 @@
         <xdr:cNvPr id="4" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2377,7 +2376,7 @@
         <xdr:cNvPr id="5" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2472,7 +2471,7 @@
         <xdr:cNvPr id="6" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2594,7 +2593,7 @@
         <xdr:cNvPr id="7" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2689,7 +2688,7 @@
         <xdr:cNvPr id="8" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2789,7 +2788,7 @@
         <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3187,8 +3186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ28"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E3" sqref="B3:E3"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3251,7 +3250,7 @@
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>194</v>
       </c>
       <c r="F3"/>
       <c r="AMH3"/>
@@ -3289,7 +3288,7 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.15">
@@ -3890,7 +3889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
1. Modified acceptance test 2. Modified team report for sprint 2 3. Merged test cases in tree.ged
</commit_message>
<xml_diff>
--- a/TeamGZWReport.xlsx
+++ b/TeamGZWReport.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\SIT\SSW555\SSW555Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaojieli/Desktop/Spring2018/SSW555/Project/SSW555Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="15555" tabRatio="993"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" tabRatio="993" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
     <sheet name="Backlog" sheetId="2" r:id="rId2"/>
-    <sheet name="Burndown README" sheetId="3" r:id="rId3"/>
-    <sheet name="Burndown" sheetId="4" r:id="rId4"/>
-    <sheet name="Sprint1" sheetId="5" r:id="rId5"/>
-    <sheet name="Sprint2" sheetId="6" r:id="rId6"/>
-    <sheet name="Sprint3" sheetId="7" r:id="rId7"/>
-    <sheet name="Sprint4" sheetId="8" r:id="rId8"/>
-    <sheet name="Stories" sheetId="9" r:id="rId9"/>
+    <sheet name="Burndown" sheetId="4" r:id="rId3"/>
+    <sheet name="Sprint1" sheetId="5" r:id="rId4"/>
+    <sheet name="Sprint2" sheetId="6" r:id="rId5"/>
+    <sheet name="Sprint3" sheetId="7" r:id="rId6"/>
+    <sheet name="Sprint4" sheetId="8" r:id="rId7"/>
+    <sheet name="Stories" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="241">
   <si>
     <t>Initials</t>
   </si>
@@ -262,30 +261,9 @@
     <t>Marriage after 14</t>
   </si>
   <si>
-    <t>The goal of the burndown chart is to help the agile team and customer to understand how the developers are doing</t>
-  </si>
-  <si>
-    <t>to deliver the product.  Burndown charts can be done daily, weekly, at the end of a sprint, or at whatever time interval makes sense.</t>
-  </si>
-  <si>
-    <t>We'll update our burndown chart for the GEDCOM project at the end of each sprint.</t>
-  </si>
-  <si>
-    <t>At the end of each sprint, you should update the number of remaining stories, the LOC written to implement the user stories</t>
-  </si>
-  <si>
-    <t>implemented in this sprint, and the minutes needed to write those lines of code.</t>
-  </si>
-  <si>
-    <t>Here's a sample burndown chart for a team of three:</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Remaining Stories</t>
-  </si>
-  <si>
     <t>Story Velocity</t>
   </si>
   <si>
@@ -296,21 +274,6 @@
   </si>
   <si>
     <t>Code Velocity</t>
-  </si>
-  <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>Sprint 1</t>
-  </si>
-  <si>
-    <t>Sprint 2</t>
-  </si>
-  <si>
-    <t>Sprint 3</t>
-  </si>
-  <si>
-    <t>Sprint 4</t>
   </si>
   <si>
     <t>Est Size(LOC)</t>
@@ -798,16 +761,51 @@
   <si>
     <t>https://github.com/Gaojie-Li/SSW555Project/</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>T08.01</t>
+  </si>
+  <si>
+    <t>Extract birth date</t>
+  </si>
+  <si>
+    <t>T08.02</t>
+  </si>
+  <si>
+    <t>Extract parents marriage date</t>
+  </si>
+  <si>
+    <t>T08.03</t>
+  </si>
+  <si>
+    <t>Compare two dates</t>
+  </si>
+  <si>
+    <t>T09.01</t>
+  </si>
+  <si>
+    <t>T09.02</t>
+  </si>
+  <si>
+    <t>T09.03</t>
+  </si>
+  <si>
+    <t>Extract death dates for both parents</t>
+  </si>
+  <si>
+    <t>Compare all dates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
-    <numFmt numFmtId="176" formatCode="m/d"/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
-    <numFmt numFmtId="178" formatCode="m/d/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -858,18 +856,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD7E4BD"/>
-        <bgColor rgb="FFCCCCFF"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -887,17 +879,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -907,22 +896,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1006,266 +995,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <c:style val="18"/>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="4A7EBB"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="4A7EBB"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Burndown README'!$B$15:$B$20</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>41065</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41078</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41092</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41106</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41120</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Burndown README'!$C$15:$C$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F690-4477-BD90-CBFE7542BB78}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="-749505984"/>
-        <c:axId val="-736218096"/>
-      </c:lineChart>
-      <c:dateAx>
-        <c:axId val="-749505984"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="878787"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-736218096"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
-      <c:valAx>
-        <c:axId val="-736218096"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="878787"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="878787"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-749505984"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1310,6 +1042,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1335,7 +1068,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1382,10 +1115,10 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41681</c:v>
+                  <c:v>41681.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41695</c:v>
+                  <c:v>41695.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1397,16 +1130,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-65F3-44CB-887C-3143EE86AB37}"/>
             </c:ext>
@@ -1449,10 +1182,10 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41681</c:v>
+                  <c:v>41681.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41695</c:v>
+                  <c:v>41695.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1464,16 +1197,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-65F3-44CB-887C-3143EE86AB37}"/>
             </c:ext>
@@ -1489,11 +1222,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-736203104"/>
-        <c:axId val="-736201056"/>
+        <c:axId val="-773101264"/>
+        <c:axId val="-773099216"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-736203104"/>
+        <c:axId val="-773101264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1533,17 +1266,17 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-736201056"/>
+        <c:crossAx val="-773099216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-736201056"/>
+        <c:axId val="-773099216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1591,10 +1324,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-736203104"/>
+        <c:crossAx val="-773101264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1632,7 +1365,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2188,671 +1921,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>81720</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>160920</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>397440</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>469080</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>25560</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>947880</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CustomShape 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1335600" y="1511280"/>
-          <a:ext cx="1231200" cy="630360"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 63937"/>
-            <a:gd name="adj2" fmla="val 85744"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="4A7EBB"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="35000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>= # team members * 4 sprints * </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:uFill>
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a:uFill>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>2 stories per sprint</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:uFill>
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a:uFill>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>113400</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>498960</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>42120</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="CustomShape 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5504400" y="1485720"/>
-          <a:ext cx="1223640" cy="537480"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -8539"/>
-            <a:gd name="adj2" fmla="val 66736"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="4A7EBB"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="35000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>lines of code per hour is calcuated by Excel</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:uFill>
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a:uFill>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1239480</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>160920</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>77040</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>135000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="CustomShape 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2858400" y="1316520"/>
-          <a:ext cx="1076040" cy="799560"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 18748"/>
-            <a:gd name="adj2" fmla="val 58438"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="4A7EBB"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="35000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Velocity of completing user stories (calculated)</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:uFill>
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a:uFill>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>111240</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>507600</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>84240</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CustomShape 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3968640" y="1638000"/>
-          <a:ext cx="396360" cy="427320"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -19786"/>
-            <a:gd name="adj2" fmla="val 63376"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="4A7EBB"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="35000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Total </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:uFill>
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a:uFill>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>LOC</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:uFill>
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a:uFill>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>20160</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>16920</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>109440</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>101160</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="CustomShape 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4420440" y="1337400"/>
-          <a:ext cx="1080000" cy="744840"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 11880"/>
-            <a:gd name="adj2" fmla="val 73902"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="4A7EBB"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="35000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>How long to implement the user stories in this sprint</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:uFill>
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a:uFill>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>265680</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>626040</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>143640</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="CustomShape 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5656680" y="5126400"/>
-          <a:ext cx="1198440" cy="630360"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -51744"/>
-            <a:gd name="adj2" fmla="val 81797"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="4A7EBB"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="35000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>When we expect to complete all user stories</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:uFill>
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a:uFill>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -2871,7 +1939,7 @@
         <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3157,16 +2225,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="15.625" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3183,7 +2251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -3200,7 +2268,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3217,7 +2285,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -3234,7 +2302,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="D9" s="1" t="s">
         <v>19</v>
       </c>
@@ -3242,13 +2310,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E10" s="18" t="s">
-        <v>240</v>
-      </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="E10" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3270,16 +2338,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -3299,7 +2367,7 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3313,14 +2381,14 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="F2"/>
       <c r="AMH2"/>
       <c r="AMI2"/>
       <c r="AMJ2"/>
     </row>
-    <row r="3" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3334,14 +2402,14 @@
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="F3"/>
       <c r="AMH3"/>
       <c r="AMI3"/>
       <c r="AMJ3"/>
     </row>
-    <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3349,16 +2417,16 @@
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3366,16 +2434,16 @@
         <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3389,10 +2457,10 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3400,30 +2468,33 @@
         <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:1024" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>2</v>
       </c>
@@ -3436,8 +2507,11 @@
       <c r="D10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:1024" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>2</v>
       </c>
@@ -3451,38 +2525,44 @@
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1024" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:1024" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>134</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>135</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:1024" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2</v>
       </c>
@@ -3496,10 +2576,10 @@
         <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1024" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>3</v>
       </c>
@@ -3513,7 +2593,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>3</v>
       </c>
@@ -3527,7 +2607,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>3</v>
       </c>
@@ -3541,7 +2621,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>3</v>
       </c>
@@ -3555,7 +2635,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>3</v>
       </c>
@@ -3569,7 +2649,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>3</v>
       </c>
@@ -3583,7 +2663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>4</v>
       </c>
@@ -3597,7 +2677,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>4</v>
       </c>
@@ -3611,7 +2691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>4</v>
       </c>
@@ -3625,7 +2705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>4</v>
       </c>
@@ -3639,7 +2719,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>4</v>
       </c>
@@ -3653,7 +2733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>4</v>
       </c>
@@ -3676,244 +2756,47 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="8.875" style="3"/>
-    <col min="6" max="6" width="8.875" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F5"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8"/>
-    </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B15" s="7">
-        <v>41065</v>
-      </c>
-      <c r="C15" s="8">
-        <v>24</v>
-      </c>
-      <c r="E15" s="8">
-        <v>0</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" s="7">
-        <v>41078</v>
-      </c>
-      <c r="C16" s="8">
-        <v>18</v>
-      </c>
-      <c r="D16">
-        <f>C15-C16</f>
-        <v>6</v>
-      </c>
-      <c r="E16" s="8">
-        <v>250</v>
-      </c>
-      <c r="F16" s="8">
-        <v>120</v>
-      </c>
-      <c r="G16" s="4">
-        <f>(E16-E15)/F16*60</f>
-        <v>125.00000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" s="7">
-        <v>41092</v>
-      </c>
-      <c r="C17" s="8">
-        <v>12</v>
-      </c>
-      <c r="D17">
-        <f>C16-C17</f>
-        <v>6</v>
-      </c>
-      <c r="E17" s="8">
-        <v>480</v>
-      </c>
-      <c r="F17" s="9">
-        <v>135</v>
-      </c>
-      <c r="G17" s="4">
-        <f>(E17-E16)/F17*60</f>
-        <v>102.22222222222223</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B18" s="7">
-        <v>41106</v>
-      </c>
-      <c r="C18" s="8">
-        <v>6</v>
-      </c>
-      <c r="D18">
-        <f>C17-C18</f>
-        <v>6</v>
-      </c>
-      <c r="E18" s="8">
-        <v>740</v>
-      </c>
-      <c r="F18" s="9">
-        <v>160</v>
-      </c>
-      <c r="G18" s="4">
-        <f>(E18-E17)/F18*60</f>
-        <v>97.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B19" s="7">
-        <v>41120</v>
-      </c>
-      <c r="C19" s="8">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <f>C18-C19</f>
-        <v>6</v>
-      </c>
-      <c r="E19" s="8">
-        <v>1100</v>
-      </c>
-      <c r="F19" s="9">
-        <v>145</v>
-      </c>
-      <c r="G19" s="4">
-        <f>(E19-E18)/F19*60</f>
-        <v>148.9655172413793</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="20.5" style="3" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.375" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="15.125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>41681</v>
       </c>
@@ -3928,7 +2811,7 @@
       </c>
       <c r="G2"/>
     </row>
-    <row r="3" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>41695</v>
       </c>
@@ -3955,16 +2838,16 @@
         <v>32.857142857142861</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B7"/>
     </row>
   </sheetData>
@@ -3975,29 +2858,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="26.125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="15.125" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="17.625" customWidth="1"/>
-    <col min="8" max="8" width="17.875" customWidth="1"/>
-    <col min="9" max="9" width="19.875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -4006,28 +2889,28 @@
       <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E1" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="I2" s="5">
         <v>41695</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -4038,7 +2921,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="E3" s="1">
         <v>50</v>
@@ -4052,47 +2935,47 @@
       <c r="H3" s="1">
         <v>50</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
       <c r="I6"/>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -4103,7 +2986,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="E7" s="1">
         <v>40</v>
@@ -4117,62 +3000,62 @@
       <c r="H7" s="1">
         <v>30</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B11"/>
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="E12" s="1">
         <v>15</v>
@@ -4187,18 +3070,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>190</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>191</v>
+        <v>178</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>179</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="E13">
         <v>12</v>
@@ -4213,18 +3096,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>193</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>194</v>
+        <v>181</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>182</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="E14">
         <v>12</v>
@@ -4239,18 +3122,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>195</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>196</v>
+        <v>183</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>184</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="E15">
         <v>3</v>
@@ -4265,18 +3148,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="E17" s="1">
         <v>15</v>
@@ -4292,18 +3175,18 @@
       </c>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>197</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>198</v>
+        <v>185</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>186</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="E18">
         <v>11</v>
@@ -4318,18 +3201,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>199</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>200</v>
+        <v>187</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>188</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="E19">
         <v>11</v>
@@ -4344,18 +3227,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>201</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>202</v>
+        <v>189</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>190</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="E20">
         <v>4</v>
@@ -4370,18 +3253,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="E22" s="1">
         <v>30</v>
@@ -4397,23 +3280,23 @@
       </c>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>203</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>205</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
@@ -4424,7 +3307,7 @@
         <v>15</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="E26" s="1">
         <v>30</v>
@@ -4440,50 +3323,419 @@
       </c>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>207</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="39" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>209</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="32.5" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B2" s="7"/>
+      <c r="I2" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E3" s="1">
+        <v>100</v>
+      </c>
+      <c r="F3" s="1">
+        <v>120</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="12"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A6" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E6" s="1">
+        <v>80</v>
+      </c>
+      <c r="F6" s="1">
+        <v>60</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>183</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B14" s="7"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>185</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>189</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B19" s="7"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E20" s="1">
+        <v>50</v>
+      </c>
+      <c r="F20" s="1">
+        <v>60</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>230</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>232</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="B23" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B24" s="7"/>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E25" s="1">
+        <v>50</v>
+      </c>
+      <c r="F25" s="1">
+        <v>60</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="B26" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="B27" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>239</v>
+      <c r="B28" s="7" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -4495,29 +3747,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="23.875" customWidth="1"/>
-    <col min="3" max="3" width="11.125" customWidth="1"/>
-    <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="17.25" customWidth="1"/>
-    <col min="6" max="6" width="21.125" customWidth="1"/>
-    <col min="7" max="7" width="16.125" customWidth="1"/>
-    <col min="8" max="8" width="21.25" customWidth="1"/>
-    <col min="9" max="9" width="17.25" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -4526,305 +3768,21 @@
       <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="10"/>
-      <c r="I2" s="5" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="E3" s="1">
-        <v>100</v>
-      </c>
-      <c r="F3" s="1">
-        <v>120</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="15"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>223</v>
-      </c>
-      <c r="B4" t="s">
-        <v>226</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>224</v>
-      </c>
-      <c r="B5" t="s">
-        <v>225</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="E6" s="1">
-        <v>80</v>
-      </c>
-      <c r="F6" s="1">
-        <v>60</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>227</v>
-      </c>
-      <c r="B7" t="s">
-        <v>229</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>228</v>
-      </c>
-      <c r="B8" t="s">
-        <v>230</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>190</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>193</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>195</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="10"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>197</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>199</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>201</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="10"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="5"/>
-    </row>
-    <row r="21" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>203</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>205</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B23" s="10"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>207</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>209</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="I26" s="3"/>
+      <c r="E1" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -4841,13 +3799,13 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -4856,20 +3814,20 @@
       <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>93</v>
+      <c r="E1" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -4881,535 +3839,489 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="251.875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="251.83203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>46</v>
       </c>
       <c r="B3" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>44</v>
       </c>
       <c r="B4" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>36</v>
       </c>
       <c r="B5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C5" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>34</v>
       </c>
       <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C6" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>50</v>
       </c>
       <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C7" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C8" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>52</v>
       </c>
       <c r="B9" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C9" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>58</v>
       </c>
       <c r="B10" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C10" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>72</v>
       </c>
       <c r="B11" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C11" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="B13" t="s">
-        <v>125</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>60</v>
       </c>
       <c r="B14" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C14" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B15" t="s">
-        <v>129</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s">
-        <v>132</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>70</v>
       </c>
       <c r="B17" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C17" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>64</v>
       </c>
       <c r="B18" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C18" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>66</v>
       </c>
       <c r="B19" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>128</v>
+      </c>
+      <c r="B21" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
         <v>137</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B24" t="s">
         <v>138</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C24" s="11" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
         <v>140</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B25" t="s">
         <v>141</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C25" s="11" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
         <v>143</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B26" t="s">
         <v>144</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C26" s="11" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>146</v>
-      </c>
-      <c r="B23" t="s">
-        <v>147</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>149</v>
-      </c>
-      <c r="B24" t="s">
-        <v>150</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>152</v>
-      </c>
-      <c r="B25" t="s">
-        <v>153</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>155</v>
-      </c>
-      <c r="B26" t="s">
-        <v>156</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>32</v>
       </c>
       <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="14" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C27" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>38</v>
       </c>
       <c r="B28" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="14" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C28" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>42</v>
       </c>
       <c r="B29" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="14" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C29" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>40</v>
       </c>
       <c r="B30" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C30" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B31" t="s">
-        <v>163</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>54</v>
       </c>
       <c r="B32" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" t="s">
+        <v>155</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" t="s">
+        <v>158</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>160</v>
+      </c>
+      <c r="B35" t="s">
+        <v>161</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>163</v>
+      </c>
+      <c r="B36" t="s">
+        <v>164</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
         <v>166</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B37" t="s">
         <v>167</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C37" s="11" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
         <v>169</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B38" t="s">
         <v>170</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C38" s="11" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>172</v>
-      </c>
-      <c r="B35" t="s">
-        <v>173</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>175</v>
-      </c>
-      <c r="B36" t="s">
-        <v>176</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>178</v>
-      </c>
-      <c r="B37" t="s">
-        <v>179</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>181</v>
-      </c>
-      <c r="B38" t="s">
-        <v>182</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>62</v>
       </c>
       <c r="B39" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="14" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C39" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>68</v>
       </c>
       <c r="B40" t="s">
         <v>69</v>
       </c>
-      <c r="C40" s="14" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C40" s="11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>26</v>
       </c>
       <c r="B41" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="14" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C41" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>48</v>
       </c>
       <c r="B42" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="14" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C42" s="11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>28</v>
       </c>
       <c r="B43" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="14" t="s">
-        <v>188</v>
+      <c r="C43" s="11" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add ZL plans for sprint2
</commit_message>
<xml_diff>
--- a/TeamGZWReport.xlsx
+++ b/TeamGZWReport.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaojieli/Desktop/Spring2018/SSW555/Project/SSW555Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizheng/Desktop/SSW555/SSW555Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" tabRatio="993" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="993" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="249">
   <si>
     <t>Initials</t>
   </si>
@@ -797,6 +797,30 @@
   </si>
   <si>
     <t>Compare all dates</t>
+  </si>
+  <si>
+    <t>T22.01</t>
+  </si>
+  <si>
+    <t>parse all IDs</t>
+  </si>
+  <si>
+    <t>T22.02</t>
+  </si>
+  <si>
+    <t>find duplicates</t>
+  </si>
+  <si>
+    <t>T29.01</t>
+  </si>
+  <si>
+    <t>determine sort standard</t>
+  </si>
+  <si>
+    <t>T29.02</t>
+  </si>
+  <si>
+    <t>sort</t>
   </si>
 </sst>
 </file>
@@ -1222,11 +1246,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-773101264"/>
-        <c:axId val="-773099216"/>
+        <c:axId val="-910260320"/>
+        <c:axId val="-812486560"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-773101264"/>
+        <c:axId val="-910260320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1269,14 +1293,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773099216"/>
+        <c:crossAx val="-812486560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-773099216"/>
+        <c:axId val="-812486560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1327,7 +1351,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773101264"/>
+        <c:crossAx val="-910260320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1939,7 +1963,7 @@
         <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2862,7 +2886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -3378,10 +3402,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3523,27 +3547,33 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>134</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E10" s="1">
+        <v>30</v>
+      </c>
+      <c r="F10" s="1">
+        <v>30</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>178</v>
+        <v>241</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>179</v>
+        <v>242</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -3552,55 +3582,61 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>181</v>
+        <v>243</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>182</v>
+        <v>244</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="26" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>183</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B13" s="7"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B14" s="7"/>
-      <c r="I14" s="3"/>
+      <c r="D14" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E14" s="1">
+        <v>15</v>
+      </c>
+      <c r="F14" s="1">
+        <v>20</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="A15" t="s">
+        <v>245</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C15" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" ht="26" x14ac:dyDescent="0.15">
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>185</v>
+        <v>247</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>186</v>
+        <v>248</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -3608,133 +3644,109 @@
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
-        <v>187</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
+      <c r="B17" s="7"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" ht="26" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>189</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" s="3"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E18" s="1">
+        <v>50</v>
+      </c>
+      <c r="F18" s="1">
+        <v>60</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B19" s="7"/>
+      <c r="A19" t="s">
+        <v>230</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="E20" s="1">
-        <v>50</v>
-      </c>
-      <c r="F20" s="1">
-        <v>60</v>
-      </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="5"/>
+      <c r="A20" t="s">
+        <v>232</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B22" s="7"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E23" s="1">
+        <v>50</v>
+      </c>
+      <c r="F23" s="1">
+        <v>60</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>236</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
-        <v>232</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
-        <v>234</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B24" s="7"/>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A25" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="E25" s="1">
-        <v>50</v>
-      </c>
-      <c r="F25" s="1">
-        <v>60</v>
-      </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="5"/>
+      <c r="A25" t="s">
+        <v>237</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A27" t="s">
-        <v>237</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A28" t="s">
-        <v>238</v>
-      </c>
-      <c r="B28" s="7" t="s">
         <v>240</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change test output to file. Run AcceptanceTest to get the result file.
</commit_message>
<xml_diff>
--- a/TeamGZWReport.xlsx
+++ b/TeamGZWReport.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizheng/Desktop/SSW555/SSW555Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaojieli/Desktop/Spring2018/SSW555/Project/SSW555Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="993" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" tabRatio="993" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -755,10 +755,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>N/A</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>https://github.com/Gaojie-Li/SSW555Project/</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -821,6 +817,9 @@
   </si>
   <si>
     <t>sort</t>
+  </si>
+  <si>
+    <t>We didn't using pair programming in implementing user stories for the first sprint which we should start using it for all future sprint.</t>
   </si>
 </sst>
 </file>
@@ -1246,11 +1245,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-910260320"/>
-        <c:axId val="-812486560"/>
+        <c:axId val="-717969632"/>
+        <c:axId val="-717967584"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-910260320"/>
+        <c:axId val="-717969632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1293,14 +1292,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-812486560"/>
+        <c:crossAx val="-717967584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-812486560"/>
+        <c:axId val="-717967584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1351,7 +1350,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-910260320"/>
+        <c:crossAx val="-717969632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1963,7 +1962,7 @@
         <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2336,7 +2335,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="E10" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
@@ -2515,7 +2514,7 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:1024" x14ac:dyDescent="0.15">
@@ -2532,7 +2531,7 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:1024" x14ac:dyDescent="0.15">
@@ -2566,7 +2565,7 @@
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:1024" x14ac:dyDescent="0.15">
@@ -2583,7 +2582,7 @@
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:1024" x14ac:dyDescent="0.15">
@@ -2886,8 +2885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3390,7 +3389,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>227</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -3404,7 +3403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -3556,7 +3555,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E10" s="1">
         <v>30</v>
@@ -3570,10 +3569,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
+        <v>240</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>241</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>242</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -3582,10 +3581,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
+        <v>242</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>243</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>244</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -3607,7 +3606,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E14" s="1">
         <v>15</v>
@@ -3621,10 +3620,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>245</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>246</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -3633,10 +3632,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
+        <v>246</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>247</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>248</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -3658,7 +3657,7 @@
         <v>15</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E18" s="1">
         <v>50</v>
@@ -3672,28 +3671,28 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
+        <v>229</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>230</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>231</v>
       </c>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
+        <v>231</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>232</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>233</v>
       </c>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
+        <v>233</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>234</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>235</v>
       </c>
       <c r="I21" s="3"/>
     </row>
@@ -3712,7 +3711,7 @@
         <v>15</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E23" s="1">
         <v>50</v>
@@ -3726,28 +3725,28 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated sprint2 stuff from Gaojie
</commit_message>
<xml_diff>
--- a/TeamGZWReport.xlsx
+++ b/TeamGZWReport.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\SIT\SSW555\SSW555Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaojieli/Desktop/Spring2018/SSW555/Project/SSW555Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="15555" tabRatio="993"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" tabRatio="993" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Sprint4" sheetId="8" r:id="rId7"/>
     <sheet name="Stories" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="269">
   <si>
     <t>Initials</t>
   </si>
@@ -854,15 +854,51 @@
   <si>
     <t>SSW555Project</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Done </t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>T11.01</t>
+  </si>
+  <si>
+    <t>Extract all FAMS information</t>
+  </si>
+  <si>
+    <t>T11.02</t>
+  </si>
+  <si>
+    <t>Compare their marry date and divorce date</t>
+  </si>
+  <si>
+    <t>T11.03</t>
+  </si>
+  <si>
+    <t>Check whether any dates overlapped</t>
+  </si>
+  <si>
+    <t>T30.01</t>
+  </si>
+  <si>
+    <t>Get Birth, Death, Marry info for everyone</t>
+  </si>
+  <si>
+    <t>T30.02</t>
+  </si>
+  <si>
+    <t>List all ppl who has already married</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="m/d"/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="m/d"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -952,10 +988,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -965,7 +1001,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -983,10 +1019,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1070,9 +1106,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1117,6 +1153,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1142,7 +1179,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1189,13 +1226,13 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41681</c:v>
+                  <c:v>41681.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41695</c:v>
+                  <c:v>41695.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41716</c:v>
+                  <c:v>41716.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1207,19 +1244,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-65F3-44CB-887C-3143EE86AB37}"/>
             </c:ext>
@@ -1262,13 +1299,13 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41681</c:v>
+                  <c:v>41681.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41695</c:v>
+                  <c:v>41695.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41716</c:v>
+                  <c:v>41716.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1280,19 +1317,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-65F3-44CB-887C-3143EE86AB37}"/>
             </c:ext>
@@ -1308,11 +1345,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-717969632"/>
-        <c:axId val="-717967584"/>
+        <c:axId val="482888944"/>
+        <c:axId val="485709056"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-717969632"/>
+        <c:axId val="482888944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1352,17 +1389,17 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-717967584"/>
+        <c:crossAx val="485709056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-717967584"/>
+        <c:axId val="485709056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1410,10 +1447,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-717969632"/>
+        <c:crossAx val="482888944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1451,7 +1488,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2025,7 +2062,7 @@
         <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2311,17 +2348,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="27.625" customWidth="1"/>
-    <col min="5" max="5" width="25.25" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2338,7 +2375,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2355,7 +2392,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2372,7 +2409,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2389,7 +2426,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="D9" s="1" t="s">
         <v>18</v>
       </c>
@@ -2417,16 +2454,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ28"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C21" sqref="B21:C21"/>
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2446,7 +2483,7 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2467,7 +2504,7 @@
       <c r="AMI2"/>
       <c r="AMJ2"/>
     </row>
-    <row r="3" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2488,7 +2525,7 @@
       <c r="AMI3"/>
       <c r="AMJ3"/>
     </row>
-    <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2505,7 +2542,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2522,7 +2559,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2539,7 +2576,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2556,7 +2593,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2570,10 +2607,10 @@
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1024" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2590,7 +2627,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2607,7 +2644,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="12" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2621,10 +2658,10 @@
         <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1024" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2641,7 +2678,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="14" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2658,21 +2695,24 @@
         <v>243</v>
       </c>
     </row>
-    <row r="16" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="D16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>3</v>
       </c>
@@ -2686,7 +2726,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>3</v>
       </c>
@@ -2700,21 +2740,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>148</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>149</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2728,7 +2771,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2742,7 +2785,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>4</v>
       </c>
@@ -2756,7 +2799,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>4</v>
       </c>
@@ -2770,7 +2813,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>4</v>
       </c>
@@ -2784,7 +2827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>4</v>
       </c>
@@ -2798,7 +2841,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>4</v>
       </c>
@@ -2812,7 +2855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>4</v>
       </c>
@@ -2837,22 +2880,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="20.5" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.375" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="15.125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>72</v>
       </c>
@@ -2875,7 +2918,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>41681</v>
       </c>
@@ -2890,7 +2933,7 @@
       </c>
       <c r="G2"/>
     </row>
-    <row r="3" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>41695</v>
       </c>
@@ -2917,7 +2960,7 @@
         <v>32.857142857142861</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>41716</v>
       </c>
@@ -2930,14 +2973,26 @@
       <c r="D4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <f>33+37+28+23</f>
+        <v>121</v>
+      </c>
+      <c r="F4">
+        <f>100+200+30+30</f>
+        <v>360</v>
+      </c>
+      <c r="G4" s="4">
+        <f>E4/F4*60</f>
+        <v>20.166666666666668</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B7"/>
     </row>
   </sheetData>
@@ -2952,21 +3007,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H37" sqref="A31:H37"/>
+    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="26.125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="15.125" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="17.625" customWidth="1"/>
-    <col min="8" max="8" width="17.875" customWidth="1"/>
-    <col min="9" max="9" width="19.875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -2995,12 +3050,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="I2" s="5">
         <v>41695</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -3029,7 +3084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>80</v>
       </c>
@@ -3041,7 +3096,7 @@
       </c>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -3053,7 +3108,7 @@
       </c>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>84</v>
       </c>
@@ -3065,7 +3120,7 @@
       </c>
       <c r="I6"/>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -3094,7 +3149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -3106,7 +3161,7 @@
       </c>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>88</v>
       </c>
@@ -3118,7 +3173,7 @@
       </c>
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>90</v>
       </c>
@@ -3130,11 +3185,11 @@
       </c>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B11"/>
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -3160,7 +3215,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>176</v>
       </c>
@@ -3186,7 +3241,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>179</v>
       </c>
@@ -3212,7 +3267,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>181</v>
       </c>
@@ -3238,7 +3293,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -3265,7 +3320,7 @@
       </c>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>183</v>
       </c>
@@ -3291,7 +3346,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>185</v>
       </c>
@@ -3317,7 +3372,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>187</v>
       </c>
@@ -3343,7 +3398,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
@@ -3370,7 +3425,7 @@
       </c>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>189</v>
       </c>
@@ -3378,7 +3433,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>191</v>
       </c>
@@ -3386,7 +3441,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
@@ -3413,7 +3468,7 @@
       </c>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>193</v>
       </c>
@@ -3421,7 +3476,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="39" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>195</v>
       </c>
@@ -3429,32 +3484,32 @@
         <v>196</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>241</v>
       </c>
@@ -3470,23 +3525,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="32.5" customWidth="1"/>
-    <col min="3" max="3" width="11.125" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="17.125" customWidth="1"/>
-    <col min="6" max="6" width="21.125" customWidth="1"/>
-    <col min="7" max="7" width="16.125" customWidth="1"/>
-    <col min="8" max="8" width="21.125" customWidth="1"/>
-    <col min="9" max="9" width="17.125" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -3515,13 +3570,13 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B2" s="7"/>
       <c r="I2" s="5">
         <v>41716</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
         <v>40</v>
       </c>
@@ -3548,7 +3603,7 @@
       </c>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>208</v>
       </c>
@@ -3559,7 +3614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>209</v>
       </c>
@@ -3570,7 +3625,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -3597,7 +3652,7 @@
       </c>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>212</v>
       </c>
@@ -3608,7 +3663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>213</v>
       </c>
@@ -3619,7 +3674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>132</v>
       </c>
@@ -3642,7 +3697,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>233</v>
       </c>
@@ -3654,7 +3709,7 @@
       </c>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>235</v>
       </c>
@@ -3666,11 +3721,11 @@
       </c>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B13" s="7"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -3693,7 +3748,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>237</v>
       </c>
@@ -3705,7 +3760,7 @@
       </c>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>239</v>
       </c>
@@ -3717,11 +3772,11 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B17" s="7"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>50</v>
       </c>
@@ -3732,7 +3787,7 @@
         <v>14</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E18" s="1">
         <v>50</v>
@@ -3740,11 +3795,15 @@
       <c r="F18" s="1">
         <v>60</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="G18" s="1">
+        <v>23</v>
+      </c>
+      <c r="H18" s="1">
+        <v>30</v>
+      </c>
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>222</v>
       </c>
@@ -3753,7 +3812,7 @@
       </c>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>224</v>
       </c>
@@ -3762,7 +3821,7 @@
       </c>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>226</v>
       </c>
@@ -3771,11 +3830,11 @@
       </c>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B22" s="7"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>56</v>
       </c>
@@ -3786,7 +3845,7 @@
         <v>14</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="E23" s="1">
         <v>50</v>
@@ -3794,11 +3853,15 @@
       <c r="F23" s="1">
         <v>60</v>
       </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="G23" s="1">
+        <v>28</v>
+      </c>
+      <c r="H23" s="1">
+        <v>30</v>
+      </c>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>228</v>
       </c>
@@ -3807,7 +3870,7 @@
       </c>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>229</v>
       </c>
@@ -3816,7 +3879,7 @@
       </c>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>230</v>
       </c>
@@ -3824,7 +3887,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B29" s="15" t="s">
         <v>216</v>
       </c>
@@ -3836,7 +3899,7 @@
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B30" s="15" t="s">
         <v>244</v>
       </c>
@@ -3848,7 +3911,7 @@
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B31" s="15" t="s">
         <v>218</v>
       </c>
@@ -3860,7 +3923,7 @@
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B32" s="15" t="s">
         <v>219</v>
       </c>
@@ -3872,7 +3935,7 @@
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B33" s="15" t="s">
         <v>220</v>
       </c>
@@ -3884,7 +3947,7 @@
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B34" s="15"/>
       <c r="C34" s="16"/>
       <c r="D34" s="15"/>
@@ -3894,7 +3957,7 @@
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B35" s="15" t="s">
         <v>217</v>
       </c>
@@ -3906,7 +3969,7 @@
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B36" s="15" t="s">
         <v>245</v>
       </c>
@@ -3927,24 +3990,24 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="4" max="4" width="16.75" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="18.375" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="23.25" customWidth="1"/>
-    <col min="9" max="9" width="19.75" customWidth="1"/>
+    <col min="8" max="8" width="23.1640625" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -3973,13 +4036,13 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B2" s="7"/>
       <c r="I2" s="5" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
         <v>52</v>
       </c>
@@ -4002,7 +4065,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>208</v>
       </c>
@@ -4013,7 +4076,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>209</v>
       </c>
@@ -4024,7 +4087,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
         <v>58</v>
       </c>
@@ -4047,7 +4110,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>212</v>
       </c>
@@ -4058,7 +4121,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>213</v>
       </c>
@@ -4067,6 +4130,86 @@
       </c>
       <c r="C8" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E10" s="1">
+        <v>50</v>
+      </c>
+      <c r="F10" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>259</v>
+      </c>
+      <c r="B11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>261</v>
+      </c>
+      <c r="B12" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>263</v>
+      </c>
+      <c r="B13" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A15" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E15" s="1">
+        <v>30</v>
+      </c>
+      <c r="F15" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>265</v>
+      </c>
+      <c r="B16" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>267</v>
+      </c>
+      <c r="B17" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -4084,9 +4227,9 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -4127,16 +4270,16 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A31" sqref="A31:B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="251.875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="251.83203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -4147,7 +4290,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -4158,7 +4301,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -4169,7 +4312,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -4180,7 +4323,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -4191,7 +4334,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -4202,7 +4345,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -4213,7 +4356,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -4224,7 +4367,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -4235,7 +4378,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -4246,7 +4389,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -4257,7 +4400,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>107</v>
       </c>
@@ -4268,7 +4411,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>110</v>
       </c>
@@ -4279,7 +4422,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -4290,7 +4433,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>114</v>
       </c>
@@ -4301,7 +4444,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>117</v>
       </c>
@@ -4312,7 +4455,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -4323,7 +4466,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -4334,7 +4477,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -4345,7 +4488,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -4356,7 +4499,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -4367,7 +4510,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -4378,7 +4521,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>132</v>
       </c>
@@ -4389,7 +4532,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>135</v>
       </c>
@@ -4400,7 +4543,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>138</v>
       </c>
@@ -4411,7 +4554,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>141</v>
       </c>
@@ -4422,7 +4565,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -4433,7 +4576,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -4444,7 +4587,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -4455,7 +4598,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -4466,7 +4609,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>148</v>
       </c>
@@ -4477,7 +4620,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -4488,7 +4631,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>152</v>
       </c>
@@ -4499,7 +4642,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>155</v>
       </c>
@@ -4510,7 +4653,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>158</v>
       </c>
@@ -4521,7 +4664,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>161</v>
       </c>
@@ -4532,7 +4675,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>164</v>
       </c>
@@ -4543,7 +4686,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>167</v>
       </c>
@@ -4554,7 +4697,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -4565,7 +4708,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>66</v>
       </c>
@@ -4576,7 +4719,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -4587,7 +4730,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -4598,7 +4741,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
add  us29 and us31
</commit_message>
<xml_diff>
--- a/TeamGZWReport.xlsx
+++ b/TeamGZWReport.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaojieli/Desktop/Spring2018/SSW555/Project/SSW555Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizheng/Desktop/SSW555/SSW555Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" tabRatio="993" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="993" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="276">
   <si>
     <t>Initials</t>
   </si>
@@ -772,13 +772,7 @@
     <t>T22.01</t>
   </si>
   <si>
-    <t>parse all IDs</t>
-  </si>
-  <si>
     <t>T22.02</t>
-  </si>
-  <si>
-    <t>find duplicates</t>
   </si>
   <si>
     <t>T29.01</t>
@@ -890,6 +884,33 @@
   </si>
   <si>
     <t>List all ppl who has already married</t>
+  </si>
+  <si>
+    <t>iterate all individual</t>
+  </si>
+  <si>
+    <t>check birth date and fams</t>
+  </si>
+  <si>
+    <t>T35.01</t>
+  </si>
+  <si>
+    <t>Get birth date for everyone</t>
+  </si>
+  <si>
+    <t>T35.02</t>
+  </si>
+  <si>
+    <t>Calculate days</t>
+  </si>
+  <si>
+    <t>T36.01</t>
+  </si>
+  <si>
+    <t>T36.02</t>
+  </si>
+  <si>
+    <t>Get death date if exists</t>
   </si>
 </sst>
 </file>
@@ -984,7 +1005,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1017,6 +1038,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1345,11 +1367,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="482888944"/>
-        <c:axId val="485709056"/>
+        <c:axId val="-1439620144"/>
+        <c:axId val="-1439618096"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="482888944"/>
+        <c:axId val="-1439620144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1392,14 +1414,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="485709056"/>
+        <c:crossAx val="-1439618096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="485709056"/>
+        <c:axId val="-1439618096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1450,7 +1472,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="482888944"/>
+        <c:crossAx val="-1439620144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2062,7 +2084,7 @@
         <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2389,7 +2411,7 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
@@ -2431,10 +2453,10 @@
         <v>18</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -2497,7 +2519,7 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F2"/>
       <c r="AMH2"/>
@@ -2607,7 +2629,7 @@
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:1024" x14ac:dyDescent="0.15">
@@ -2641,7 +2663,7 @@
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:1024" x14ac:dyDescent="0.15">
@@ -2658,7 +2680,7 @@
         <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:1024" x14ac:dyDescent="0.15">
@@ -2692,7 +2714,7 @@
         <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:1024" x14ac:dyDescent="0.15">
@@ -2709,7 +2731,7 @@
         <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
@@ -2754,7 +2776,7 @@
         <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
@@ -2880,7 +2902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -3511,7 +3533,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -3526,7 +3548,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3587,7 +3609,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E3" s="1">
         <v>100</v>
@@ -3636,7 +3658,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E6" s="1">
         <v>80</v>
@@ -3679,7 +3701,7 @@
         <v>132</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>133</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
@@ -3693,8 +3715,12 @@
       <c r="F10" s="1">
         <v>30</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="G10" s="1">
+        <v>13</v>
+      </c>
+      <c r="H10" s="1">
+        <v>40</v>
+      </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
@@ -3702,7 +3728,7 @@
         <v>233</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>234</v>
+        <v>267</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -3711,10 +3737,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>236</v>
+        <v>268</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -3744,16 +3770,20 @@
       <c r="F14" s="1">
         <v>20</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="G14" s="1">
+        <v>11</v>
+      </c>
+      <c r="H14" s="1">
+        <v>35</v>
+      </c>
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -3762,10 +3792,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -3901,7 +3931,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B30" s="15" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C30" s="16"/>
       <c r="D30" s="15"/>
@@ -3971,7 +4001,7 @@
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B36" s="15" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C36" s="16"/>
       <c r="D36" s="15"/>
@@ -3990,10 +4020,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4039,7 +4069,7 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B2" s="7"/>
       <c r="I2" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -4047,13 +4077,13 @@
         <v>52</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E3" s="1">
         <v>30</v>
@@ -4070,7 +4100,7 @@
         <v>208</v>
       </c>
       <c r="B4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -4081,7 +4111,7 @@
         <v>209</v>
       </c>
       <c r="B5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -4098,7 +4128,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E6" s="1">
         <v>25</v>
@@ -4115,7 +4145,7 @@
         <v>212</v>
       </c>
       <c r="B7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -4126,7 +4156,7 @@
         <v>213</v>
       </c>
       <c r="B8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -4143,7 +4173,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E10" s="1">
         <v>50</v>
@@ -4154,26 +4184,26 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B12" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B13" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
@@ -4187,7 +4217,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E15" s="1">
         <v>30</v>
@@ -4198,18 +4228,104 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
+        <v>263</v>
+      </c>
+      <c r="B16" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
         <v>265</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
-        <v>267</v>
-      </c>
-      <c r="B17" t="s">
-        <v>268</v>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E19" s="1">
+        <v>25</v>
+      </c>
+      <c r="F19" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>269</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>271</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E23" s="1">
+        <v>25</v>
+      </c>
+      <c r="F23" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>273</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>274</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -4270,7 +4386,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:B31"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Modified plan for sprint3
</commit_message>
<xml_diff>
--- a/TeamGZWReport.xlsx
+++ b/TeamGZWReport.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizheng/Desktop/SSW555/SSW555Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaojieli/Desktop/Spring2018/SSW555/Project/SSW555Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="993" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" tabRatio="993" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="277">
   <si>
     <t>Initials</t>
   </si>
@@ -818,18 +818,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>List living single</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Get death date info</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Listing</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>Get birth date info</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -911,6 +899,18 @@
   </si>
   <si>
     <t>Get death date if exists</t>
+  </si>
+  <si>
+    <t>T034.01</t>
+  </si>
+  <si>
+    <t>T034.02</t>
+  </si>
+  <si>
+    <t>Get age of both husband and wife in every family</t>
+  </si>
+  <si>
+    <t>Compare the age to find the difference</t>
   </si>
 </sst>
 </file>
@@ -1175,7 +1175,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1367,11 +1366,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1439620144"/>
-        <c:axId val="-1439618096"/>
+        <c:axId val="-229720736"/>
+        <c:axId val="-229719376"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-1439620144"/>
+        <c:axId val="-229720736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1414,14 +1413,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1439618096"/>
+        <c:crossAx val="-229719376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-1439618096"/>
+        <c:axId val="-229719376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1472,7 +1471,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1439620144"/>
+        <c:crossAx val="-229720736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2084,7 +2083,7 @@
         <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2411,7 +2410,7 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
@@ -2453,10 +2452,10 @@
         <v>18</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -2629,7 +2628,7 @@
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:1024" x14ac:dyDescent="0.15">
@@ -2680,7 +2679,7 @@
         <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:1024" x14ac:dyDescent="0.15">
@@ -2731,7 +2730,7 @@
         <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
@@ -2776,7 +2775,7 @@
         <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
@@ -3547,7 +3546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -3728,7 +3727,7 @@
         <v>233</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -3740,7 +3739,7 @@
         <v>234</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -4023,12 +4022,12 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="37.33203125" customWidth="1"/>
+    <col min="2" max="2" width="45.5" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" customWidth="1"/>
@@ -4073,11 +4072,11 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A3" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>247</v>
+      <c r="A3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
@@ -4097,10 +4096,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>273</v>
       </c>
       <c r="B4" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -4108,10 +4107,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>209</v>
+        <v>274</v>
       </c>
       <c r="B5" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -4145,7 +4144,7 @@
         <v>212</v>
       </c>
       <c r="B7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -4156,7 +4155,7 @@
         <v>213</v>
       </c>
       <c r="B8" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -4173,7 +4172,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E10" s="1">
         <v>50</v>
@@ -4184,26 +4183,26 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B11" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B12" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B13" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
@@ -4217,7 +4216,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E15" s="1">
         <v>30</v>
@@ -4228,18 +4227,18 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B16" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B17" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
@@ -4253,7 +4252,7 @@
         <v>9</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E19" s="1">
         <v>25</v>
@@ -4264,10 +4263,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -4276,10 +4275,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -4303,7 +4302,7 @@
         <v>9</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E23" s="1">
         <v>25</v>
@@ -4314,18 +4313,18 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -4385,8 +4384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A14" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
(1) accep test: US34 & US13 (2) report update
</commit_message>
<xml_diff>
--- a/TeamGZWReport.xlsx
+++ b/TeamGZWReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="993" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="993" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="299">
   <si>
     <t>Initials</t>
   </si>
@@ -730,9 +730,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>Coding</t>
-  </si>
-  <si>
     <t>T08.01</t>
   </si>
   <si>
@@ -803,18 +800,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>2018/3/--</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>coding</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>coding</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>Get birth date info</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -959,6 +944,62 @@
   </si>
   <si>
     <t>Siblings spacing</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Marriage after 14</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>WX</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>WX</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Planning</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GL</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GL</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZL</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZL</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Done </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Planning</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018/4/--</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1304,6 +1345,9 @@
                 <c:pt idx="2">
                   <c:v>41716</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>41730</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1321,6 +1365,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1377,6 +1424,9 @@
                 <c:pt idx="2">
                   <c:v>41716</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>41730</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1394,6 +1444,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2419,7 +2472,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2459,7 +2512,7 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2501,10 +2554,10 @@
         <v>18</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2524,8 +2577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2567,7 +2620,7 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F2"/>
       <c r="AMH2"/>
@@ -2677,7 +2730,7 @@
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:1024" x14ac:dyDescent="0.2">
@@ -2694,7 +2747,7 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>220</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:1024" x14ac:dyDescent="0.2">
@@ -2711,7 +2764,7 @@
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:1024" x14ac:dyDescent="0.2">
@@ -2728,7 +2781,7 @@
         <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:1024" x14ac:dyDescent="0.2">
@@ -2745,7 +2798,7 @@
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>220</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:1024" x14ac:dyDescent="0.2">
@@ -2762,7 +2815,7 @@
         <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:1024" x14ac:dyDescent="0.2">
@@ -2778,19 +2831,16 @@
       <c r="D16" t="s">
         <v>14</v>
       </c>
-      <c r="E16" t="s">
-        <v>252</v>
-      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C17" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
@@ -2801,13 +2851,16 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C18" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -2823,19 +2876,16 @@
       <c r="D19" t="s">
         <v>14</v>
       </c>
-      <c r="E19" t="s">
-        <v>252</v>
-      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C20" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
@@ -2854,6 +2904,9 @@
       <c r="D21" t="s">
         <v>5</v>
       </c>
+      <c r="E21" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
@@ -2868,6 +2921,9 @@
       <c r="D23" t="s">
         <v>14</v>
       </c>
+      <c r="E23" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
@@ -2882,6 +2938,9 @@
       <c r="D24" t="s">
         <v>9</v>
       </c>
+      <c r="E24" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
@@ -2896,6 +2955,9 @@
       <c r="D25" t="s">
         <v>5</v>
       </c>
+      <c r="E25" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
@@ -2910,6 +2972,9 @@
       <c r="D26" t="s">
         <v>14</v>
       </c>
+      <c r="E26" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -2924,6 +2989,9 @@
       <c r="D27" t="s">
         <v>9</v>
       </c>
+      <c r="E27" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
@@ -2937,6 +3005,9 @@
       </c>
       <c r="D28" t="s">
         <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -2951,7 +3022,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3057,7 +3128,18 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B5"/>
+      <c r="A5" s="3">
+        <v>41730</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6"/>
@@ -3077,7 +3159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -3581,7 +3663,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -3596,7 +3678,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3657,7 +3739,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E3" s="1">
         <v>100</v>
@@ -3706,7 +3788,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E6" s="1">
         <v>80</v>
@@ -3746,7 +3828,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>53</v>
@@ -3773,10 +3855,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -3785,10 +3867,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -3828,10 +3910,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>233</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>234</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>235</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -3840,10 +3922,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>235</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>236</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>237</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -3883,28 +3965,28 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>220</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>221</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>222</v>
       </c>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>222</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>223</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>224</v>
       </c>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>224</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>225</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>226</v>
       </c>
       <c r="I21" s="3"/>
     </row>
@@ -3941,28 +4023,28 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -3979,7 +4061,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B30" s="15" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C30" s="16"/>
       <c r="D30" s="15"/>
@@ -4049,7 +4131,7 @@
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C36" s="16"/>
       <c r="D36" s="15"/>
@@ -4068,10 +4150,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4116,8 +4198,8 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="7"/>
-      <c r="I2" s="5" t="s">
-        <v>243</v>
+      <c r="I2" s="5">
+        <v>41730</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -4125,13 +4207,13 @@
         <v>158</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>244</v>
+        <v>196</v>
       </c>
       <c r="E3" s="1">
         <v>30</v>
@@ -4139,16 +4221,20 @@
       <c r="F3" s="1">
         <v>60</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="G3" s="1">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1">
+        <v>80</v>
+      </c>
       <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B4" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -4156,10 +4242,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B5" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -4176,7 +4262,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>245</v>
+        <v>287</v>
       </c>
       <c r="E6" s="1">
         <v>25</v>
@@ -4184,16 +4270,20 @@
       <c r="F6" s="1">
         <v>60</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="G6" s="1">
+        <v>34</v>
+      </c>
+      <c r="H6" s="1">
+        <v>100</v>
+      </c>
       <c r="I6" s="12"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B7" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -4201,13 +4291,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B8" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C8" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -4221,7 +4311,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E10" s="1">
         <v>50</v>
@@ -4232,96 +4322,108 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B11" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B12" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B13" t="s">
-        <v>258</v>
+        <v>254</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E14" s="1">
+        <v>30</v>
+      </c>
+      <c r="F14" s="1">
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="E15" s="1">
-        <v>30</v>
-      </c>
-      <c r="F15" s="1">
-        <v>60</v>
+      <c r="A15" t="s">
+        <v>255</v>
+      </c>
+      <c r="B15" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B16" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E18" s="1">
+        <v>25</v>
+      </c>
+      <c r="F18" s="1">
+        <v>60</v>
+      </c>
+      <c r="G18" s="13">
+        <v>36</v>
+      </c>
+      <c r="H18" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>261</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" s="18" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E19" s="1">
-        <v>25</v>
-      </c>
-      <c r="F19" s="1">
-        <v>60</v>
-      </c>
-      <c r="G19" s="13">
-        <v>36</v>
-      </c>
-      <c r="H19" s="1">
-        <v>70</v>
-      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -4329,63 +4431,45 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E21" s="1">
+        <v>25</v>
+      </c>
+      <c r="F21" s="1">
+        <v>60</v>
+      </c>
+      <c r="G21" s="13">
+        <v>36</v>
+      </c>
+      <c r="H21" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>265</v>
+      </c>
+      <c r="B22" s="18" t="s">
         <v>267</v>
       </c>
-      <c r="B21" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E23" s="1">
-        <v>25</v>
-      </c>
-      <c r="F23" s="1">
-        <v>60</v>
-      </c>
-      <c r="G23" s="13">
-        <v>36</v>
-      </c>
-      <c r="H23" s="1">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>269</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>270</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>268</v>
+      <c r="A23" t="s">
+        <v>266</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -4397,13 +4481,22 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="13.625" customWidth="1"/>
+    <col min="6" max="6" width="15.25" customWidth="1"/>
+    <col min="7" max="7" width="13.75" customWidth="1"/>
+    <col min="8" max="8" width="13.125" customWidth="1"/>
+    <col min="9" max="9" width="15.25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -4433,6 +4526,133 @@
       <c r="I1" s="9" t="s">
         <v>79</v>
       </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="E3" s="13">
+        <v>50</v>
+      </c>
+      <c r="F3" s="13">
+        <v>100</v>
+      </c>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="E6" s="13">
+        <v>30</v>
+      </c>
+      <c r="F6" s="13">
+        <v>60</v>
+      </c>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -4445,7 +4665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -4603,7 +4823,7 @@
         <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>113</v>
@@ -4834,7 +5054,7 @@
         <v>158</v>
       </c>
       <c r="B35" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>159</v>

</xml_diff>

<commit_message>
1. Implement US11, US30 2. Add a is_before method to simplify the code 3. Update team report
</commit_message>
<xml_diff>
--- a/TeamGZWReport.xlsx
+++ b/TeamGZWReport.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\SIT\SSW555\SSW555Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaojieli/Desktop/Spring2018/SSW555/Project/SSW555Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="993" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="21160" tabRatio="993" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Sprint4" sheetId="8" r:id="rId7"/>
     <sheet name="Stories" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="315">
   <si>
     <t>Initials</t>
   </si>
@@ -823,151 +823,172 @@
     <t xml:space="preserve">Done </t>
   </si>
   <si>
+    <t>T11.01</t>
+  </si>
+  <si>
+    <t>Extract all FAMS information</t>
+  </si>
+  <si>
+    <t>T11.02</t>
+  </si>
+  <si>
+    <t>Compare their marry date and divorce date</t>
+  </si>
+  <si>
+    <t>T11.03</t>
+  </si>
+  <si>
+    <t>Check whether any dates overlapped</t>
+  </si>
+  <si>
+    <t>T30.01</t>
+  </si>
+  <si>
+    <t>Get Birth, Death, Marry info for everyone</t>
+  </si>
+  <si>
+    <t>T30.02</t>
+  </si>
+  <si>
+    <t>List all ppl who has already married</t>
+  </si>
+  <si>
+    <t>iterate all individual</t>
+  </si>
+  <si>
+    <t>check birth date and fams</t>
+  </si>
+  <si>
+    <t>T35.01</t>
+  </si>
+  <si>
+    <t>Get birth date for everyone</t>
+  </si>
+  <si>
+    <t>T35.02</t>
+  </si>
+  <si>
+    <t>Calculate days</t>
+  </si>
+  <si>
+    <t>T36.01</t>
+  </si>
+  <si>
+    <t>T36.02</t>
+  </si>
+  <si>
+    <t>Get death date if exists</t>
+  </si>
+  <si>
+    <t>T034.01</t>
+  </si>
+  <si>
+    <t>T034.02</t>
+  </si>
+  <si>
+    <t>Get age of both husband and wife in every family</t>
+  </si>
+  <si>
+    <t>Compare the age to find the difference</t>
+  </si>
+  <si>
+    <t>US31</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>US34</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>List large age differences</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>List large age differences</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>US35</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>List recent births</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>US36</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>List recent deaths</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>WX</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>T013.01</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>T013.02</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>List large age differences</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Siblings spacing</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Marriage after 14</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>WX</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>WX</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
     <t>Planning</t>
-  </si>
-  <si>
-    <t>T11.01</t>
-  </si>
-  <si>
-    <t>Extract all FAMS information</t>
-  </si>
-  <si>
-    <t>T11.02</t>
-  </si>
-  <si>
-    <t>Compare their marry date and divorce date</t>
-  </si>
-  <si>
-    <t>T11.03</t>
-  </si>
-  <si>
-    <t>Check whether any dates overlapped</t>
-  </si>
-  <si>
-    <t>T30.01</t>
-  </si>
-  <si>
-    <t>Get Birth, Death, Marry info for everyone</t>
-  </si>
-  <si>
-    <t>T30.02</t>
-  </si>
-  <si>
-    <t>List all ppl who has already married</t>
-  </si>
-  <si>
-    <t>iterate all individual</t>
-  </si>
-  <si>
-    <t>check birth date and fams</t>
-  </si>
-  <si>
-    <t>T35.01</t>
-  </si>
-  <si>
-    <t>Get birth date for everyone</t>
-  </si>
-  <si>
-    <t>T35.02</t>
-  </si>
-  <si>
-    <t>Calculate days</t>
-  </si>
-  <si>
-    <t>T36.01</t>
-  </si>
-  <si>
-    <t>T36.02</t>
-  </si>
-  <si>
-    <t>Get death date if exists</t>
-  </si>
-  <si>
-    <t>T034.01</t>
-  </si>
-  <si>
-    <t>T034.02</t>
-  </si>
-  <si>
-    <t>Get age of both husband and wife in every family</t>
-  </si>
-  <si>
-    <t>Compare the age to find the difference</t>
-  </si>
-  <si>
-    <t>US31</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>US34</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>List large age differences</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>List large age differences</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>US35</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>List recent births</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>US36</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>List recent deaths</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>WX</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>T013.01</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>T013.02</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>List large age differences</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Siblings spacing</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Done</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Done</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Done</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Marriage after 14</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>WX</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>WX</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GL</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GL</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZL</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZL</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Done </t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -975,41 +996,68 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>GL</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>GL</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZL</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZL</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Done </t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Planning</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>2018/4/--</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>T33.01</t>
+  </si>
+  <si>
+    <t>Find everyone with 'FAMC' entry</t>
+  </si>
+  <si>
+    <t>T33.02</t>
+  </si>
+  <si>
+    <t>Check their birth date</t>
+  </si>
+  <si>
+    <t>T33.03</t>
+  </si>
+  <si>
+    <t>Check their parents living or not</t>
+  </si>
+  <si>
+    <t>T33.04</t>
+  </si>
+  <si>
+    <t>Output indivisual satisfying the condition</t>
+  </si>
+  <si>
+    <t>US21.01</t>
+  </si>
+  <si>
+    <t>Check all individuals with 'FAMS' entry</t>
+  </si>
+  <si>
+    <t>US21.02</t>
+  </si>
+  <si>
+    <t>Check their gender and their role in the family</t>
+  </si>
+  <si>
+    <t>US21.03</t>
+  </si>
+  <si>
+    <t>Report all un-corresponding entries</t>
+  </si>
+  <si>
+    <t>Using VSCode and GitHub</t>
+  </si>
+  <si>
+    <t>Efficient communication between team members</t>
+  </si>
+  <si>
+    <t>We think we are all in pretty good shape :)))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="m/d"/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="m/d"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -1089,9 +1137,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -1099,10 +1152,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1112,7 +1165,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1130,11 +1183,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="3" builtinId="9" hidden="1"/>
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1218,9 +1276,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1265,6 +1323,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1290,7 +1349,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1337,16 +1396,16 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41681</c:v>
+                  <c:v>41681.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41695</c:v>
+                  <c:v>41695.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41716</c:v>
+                  <c:v>41716.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41730</c:v>
+                  <c:v>41730.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1358,22 +1417,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-65F3-44CB-887C-3143EE86AB37}"/>
             </c:ext>
@@ -1416,16 +1475,16 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41681</c:v>
+                  <c:v>41681.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41695</c:v>
+                  <c:v>41695.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41716</c:v>
+                  <c:v>41716.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41730</c:v>
+                  <c:v>41730.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1437,22 +1496,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-65F3-44CB-887C-3143EE86AB37}"/>
             </c:ext>
@@ -1468,11 +1527,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-229720736"/>
-        <c:axId val="-229719376"/>
+        <c:axId val="-936755056"/>
+        <c:axId val="-936753008"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-229720736"/>
+        <c:axId val="-936755056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1512,17 +1571,17 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-229719376"/>
+        <c:crossAx val="-936753008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-229719376"/>
+        <c:axId val="-936753008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1570,10 +1629,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-229720736"/>
+        <c:crossAx val="-936755056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1611,7 +1670,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2185,7 +2244,7 @@
         <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2475,13 +2534,13 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="27.625" customWidth="1"/>
-    <col min="5" max="5" width="25.125" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2498,7 +2557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2515,7 +2574,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2532,7 +2591,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2549,7 +2608,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="D9" s="1" t="s">
         <v>18</v>
       </c>
@@ -2581,12 +2640,12 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2606,7 +2665,7 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2627,7 +2686,7 @@
       <c r="AMI2"/>
       <c r="AMJ2"/>
     </row>
-    <row r="3" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2648,7 +2707,7 @@
       <c r="AMI3"/>
       <c r="AMJ3"/>
     </row>
-    <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2665,7 +2724,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2682,7 +2741,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2699,7 +2758,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2716,7 +2775,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2733,7 +2792,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2747,10 +2806,10 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1024" x14ac:dyDescent="0.2">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2767,7 +2826,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="12" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2784,7 +2843,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="13" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2801,7 +2860,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="14" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2818,7 +2877,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="16" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>3</v>
       </c>
@@ -2832,38 +2891,38 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>3</v>
       </c>
       <c r="B17" t="s">
+        <v>275</v>
+      </c>
+      <c r="C17" t="s">
         <v>276</v>
-      </c>
-      <c r="C17" t="s">
-        <v>277</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2877,21 +2936,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>3</v>
       </c>
       <c r="B20" t="s">
+        <v>277</v>
+      </c>
+      <c r="C20" t="s">
         <v>278</v>
-      </c>
-      <c r="C20" t="s">
-        <v>279</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2905,10 +2964,10 @@
         <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>4</v>
       </c>
@@ -2922,10 +2981,10 @@
         <v>14</v>
       </c>
       <c r="E23" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>4</v>
       </c>
@@ -2939,10 +2998,10 @@
         <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>4</v>
       </c>
@@ -2956,10 +3015,10 @@
         <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>4</v>
       </c>
@@ -2973,10 +3032,10 @@
         <v>14</v>
       </c>
       <c r="E26" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>4</v>
       </c>
@@ -2990,10 +3049,10 @@
         <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>4</v>
       </c>
@@ -3007,7 +3066,7 @@
         <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -3022,21 +3081,21 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="26.375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.375" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="15.125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>72</v>
       </c>
@@ -3059,7 +3118,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>41681</v>
       </c>
@@ -3074,7 +3133,7 @@
       </c>
       <c r="G2"/>
     </row>
-    <row r="3" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>41695</v>
       </c>
@@ -3101,7 +3160,7 @@
         <v>32.857142857142861</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>41716</v>
       </c>
@@ -3115,19 +3174,19 @@
         <v>6</v>
       </c>
       <c r="E4">
-        <f>33+37+28+23</f>
-        <v>121</v>
+        <f>33+37+28+23+13+11</f>
+        <v>145</v>
       </c>
       <c r="F4">
-        <f>100+200+30+30</f>
-        <v>360</v>
+        <f>100+200+30+30+40+35</f>
+        <v>435</v>
       </c>
       <c r="G4" s="4">
         <f>E4/F4*60</f>
-        <v>20.166666666666668</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>41730</v>
       </c>
@@ -3140,11 +3199,23 @@
       <c r="D5">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <f>30+34+33+11+36+36</f>
+        <v>180</v>
+      </c>
+      <c r="F5">
+        <f>80+100+50+30+70+70</f>
+        <v>400</v>
+      </c>
+      <c r="G5" s="4">
+        <f>E5/F5*60</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B7"/>
     </row>
   </sheetData>
@@ -3163,17 +3234,17 @@
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="26.125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="15.125" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="17.625" customWidth="1"/>
-    <col min="8" max="8" width="17.875" customWidth="1"/>
-    <col min="9" max="9" width="19.875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -3202,12 +3273,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="I2" s="5">
         <v>41695</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -3236,7 +3307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>80</v>
       </c>
@@ -3248,7 +3319,7 @@
       </c>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -3260,7 +3331,7 @@
       </c>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>84</v>
       </c>
@@ -3272,7 +3343,7 @@
       </c>
       <c r="I6"/>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -3301,7 +3372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -3313,7 +3384,7 @@
       </c>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>88</v>
       </c>
@@ -3325,7 +3396,7 @@
       </c>
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>90</v>
       </c>
@@ -3337,11 +3408,11 @@
       </c>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B11"/>
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -3367,7 +3438,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>175</v>
       </c>
@@ -3393,7 +3464,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>178</v>
       </c>
@@ -3419,7 +3490,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>180</v>
       </c>
@@ -3445,7 +3516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -3472,7 +3543,7 @@
       </c>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>182</v>
       </c>
@@ -3498,7 +3569,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>184</v>
       </c>
@@ -3524,7 +3595,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>186</v>
       </c>
@@ -3550,7 +3621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
@@ -3577,7 +3648,7 @@
       </c>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>188</v>
       </c>
@@ -3585,7 +3656,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>190</v>
       </c>
@@ -3593,7 +3664,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
@@ -3620,7 +3691,7 @@
       </c>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>192</v>
       </c>
@@ -3628,7 +3699,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="39" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>194</v>
       </c>
@@ -3636,32 +3707,32 @@
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>237</v>
       </c>
@@ -3678,22 +3749,22 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B29" sqref="B29:H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="32.5" customWidth="1"/>
-    <col min="3" max="3" width="11.125" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="17.125" customWidth="1"/>
-    <col min="6" max="6" width="21.125" customWidth="1"/>
-    <col min="7" max="7" width="16.125" customWidth="1"/>
-    <col min="8" max="8" width="21.125" customWidth="1"/>
-    <col min="9" max="9" width="17.125" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -3722,13 +3793,13 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B2" s="7"/>
       <c r="I2" s="5">
         <v>41716</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
         <v>40</v>
       </c>
@@ -3755,7 +3826,7 @@
       </c>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>207</v>
       </c>
@@ -3766,7 +3837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>208</v>
       </c>
@@ -3777,7 +3848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -3804,7 +3875,7 @@
       </c>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>211</v>
       </c>
@@ -3815,7 +3886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>212</v>
       </c>
@@ -3826,9 +3897,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>53</v>
@@ -3853,35 +3924,35 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>231</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>232</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B13" s="7"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -3908,7 +3979,7 @@
       </c>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>233</v>
       </c>
@@ -3920,7 +3991,7 @@
       </c>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>235</v>
       </c>
@@ -3932,11 +4003,11 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B17" s="7"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>50</v>
       </c>
@@ -3963,7 +4034,7 @@
       </c>
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>220</v>
       </c>
@@ -3972,7 +4043,7 @@
       </c>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>222</v>
       </c>
@@ -3981,7 +4052,7 @@
       </c>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>224</v>
       </c>
@@ -3990,11 +4061,11 @@
       </c>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B22" s="7"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>56</v>
       </c>
@@ -4021,7 +4092,7 @@
       </c>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>226</v>
       </c>
@@ -4030,7 +4101,7 @@
       </c>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>227</v>
       </c>
@@ -4039,7 +4110,7 @@
       </c>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>228</v>
       </c>
@@ -4047,7 +4118,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B29" s="15" t="s">
         <v>215</v>
       </c>
@@ -4059,7 +4130,7 @@
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B30" s="15" t="s">
         <v>240</v>
       </c>
@@ -4071,7 +4142,7 @@
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B31" s="15" t="s">
         <v>217</v>
       </c>
@@ -4083,7 +4154,7 @@
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B32" s="15" t="s">
         <v>218</v>
       </c>
@@ -4095,7 +4166,7 @@
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B33" s="15" t="s">
         <v>219</v>
       </c>
@@ -4107,7 +4178,7 @@
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B34" s="15"/>
       <c r="C34" s="16"/>
       <c r="D34" s="15"/>
@@ -4117,7 +4188,7 @@
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B35" s="15" t="s">
         <v>216</v>
       </c>
@@ -4129,7 +4200,7 @@
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B36" s="15" t="s">
         <v>241</v>
       </c>
@@ -4144,30 +4215,30 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="45.5" customWidth="1"/>
-    <col min="4" max="4" width="16.625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="18.375" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="23.125" customWidth="1"/>
-    <col min="9" max="9" width="19.625" customWidth="1"/>
+    <col min="8" max="8" width="23.1640625" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -4196,18 +4267,18 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B2" s="7"/>
       <c r="I2" s="5">
         <v>41730</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>158</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
@@ -4229,29 +4300,29 @@
       </c>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
         <v>58</v>
       </c>
@@ -4262,7 +4333,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E6" s="1">
         <v>25</v>
@@ -4278,9 +4349,9 @@
       </c>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B7" t="s">
         <v>242</v>
@@ -4289,18 +4360,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B8" t="s">
         <v>243</v>
       </c>
       <c r="C8" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>107</v>
       </c>
@@ -4311,7 +4382,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>248</v>
+        <v>177</v>
       </c>
       <c r="E10" s="1">
         <v>50</v>
@@ -4319,32 +4390,38 @@
       <c r="F10" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G10" s="1">
+        <v>33</v>
+      </c>
+      <c r="H10" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
+        <v>248</v>
+      </c>
+      <c r="B11" t="s">
         <v>249</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>251</v>
       </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>253</v>
       </c>
-      <c r="B13" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>148</v>
       </c>
@@ -4355,7 +4432,7 @@
         <v>14</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>248</v>
+        <v>177</v>
       </c>
       <c r="E14" s="1">
         <v>30</v>
@@ -4363,24 +4440,30 @@
       <c r="F14" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G14" s="1">
+        <v>11</v>
+      </c>
+      <c r="H14" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
+        <v>254</v>
+      </c>
+      <c r="B15" t="s">
         <v>255</v>
       </c>
-      <c r="B15" t="s">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>257</v>
       </c>
-      <c r="B16" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>160</v>
       </c>
@@ -4406,31 +4489,31 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
+        <v>260</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>261</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>262</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
+        <v>262</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>263</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>264</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>163</v>
       </c>
@@ -4456,21 +4539,85 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
+        <v>264</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
         <v>265</v>
       </c>
-      <c r="B22" s="18" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>266</v>
-      </c>
       <c r="B23" s="18" t="s">
-        <v>264</v>
-      </c>
+        <v>263</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A26" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="B26" s="16"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A27" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="B27" s="16"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A28" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="B28" s="16"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A29" s="15"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A30" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B30" s="16"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A31" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="B31" s="16"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -4481,24 +4628,24 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="2" max="2" width="40.1640625" customWidth="1"/>
     <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="13.625" customWidth="1"/>
-    <col min="6" max="6" width="15.25" customWidth="1"/>
-    <col min="7" max="7" width="13.75" customWidth="1"/>
-    <col min="8" max="8" width="13.125" customWidth="1"/>
-    <col min="9" max="9" width="15.25" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -4527,12 +4674,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="I2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
         <v>64</v>
       </c>
@@ -4540,10 +4687,10 @@
         <v>65</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E3" s="13">
         <v>50</v>
@@ -4555,18 +4702,18 @@
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
         <v>70</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C6" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>290</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>291</v>
       </c>
       <c r="E6" s="13">
         <v>30</v>
@@ -4578,81 +4725,145 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="E10" s="13">
         <v>60</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
+      <c r="F10" s="13">
+        <v>100</v>
+      </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="13" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>298</v>
+      </c>
+      <c r="B11" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>300</v>
+      </c>
+      <c r="B12" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>302</v>
+      </c>
+      <c r="B13" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>304</v>
+      </c>
+      <c r="B14" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="E16" s="13">
+        <v>40</v>
+      </c>
+      <c r="F16" s="13">
+        <v>50</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>306</v>
+      </c>
+      <c r="B17" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>308</v>
+      </c>
+      <c r="B18" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>310</v>
+      </c>
+      <c r="B19" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A21" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="13" t="s">
+      <c r="D21" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A24" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
+      <c r="D24" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -4666,16 +4877,16 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A22" sqref="A22:B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="251.875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="251.83203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -4686,7 +4897,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -4697,7 +4908,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -4708,7 +4919,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -4719,7 +4930,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -4730,7 +4941,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -4741,7 +4952,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -4752,7 +4963,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -4763,7 +4974,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -4774,7 +4985,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -4785,7 +4996,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -4796,7 +5007,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>107</v>
       </c>
@@ -4807,7 +5018,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>110</v>
       </c>
@@ -4818,18 +5029,18 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>114</v>
       </c>
@@ -4840,7 +5051,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>117</v>
       </c>
@@ -4851,7 +5062,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -4862,7 +5073,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -4873,7 +5084,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -4884,7 +5095,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -4895,7 +5106,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -4906,7 +5117,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -4917,7 +5128,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>132</v>
       </c>
@@ -4928,7 +5139,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>135</v>
       </c>
@@ -4939,7 +5150,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>138</v>
       </c>
@@ -4950,7 +5161,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>141</v>
       </c>
@@ -4961,7 +5172,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -4972,7 +5183,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -4983,7 +5194,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -4994,7 +5205,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -5005,7 +5216,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>148</v>
       </c>
@@ -5016,7 +5227,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -5027,7 +5238,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>152</v>
       </c>
@@ -5038,7 +5249,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>155</v>
       </c>
@@ -5049,18 +5260,18 @@
         <v>157</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>158</v>
       </c>
       <c r="B35" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>160</v>
       </c>
@@ -5071,7 +5282,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>163</v>
       </c>
@@ -5082,7 +5293,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>166</v>
       </c>
@@ -5093,7 +5304,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -5104,7 +5315,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>66</v>
       </c>
@@ -5115,7 +5326,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -5126,7 +5337,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -5137,7 +5348,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Add us 21 and us 33 from GL.
</commit_message>
<xml_diff>
--- a/TeamGZWReport.xlsx
+++ b/TeamGZWReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="21160" tabRatio="993" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" tabRatio="993" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="317">
   <si>
     <t>Initials</t>
   </si>
@@ -1049,6 +1049,12 @@
   </si>
   <si>
     <t>We think we are all in pretty good shape :)))</t>
+  </si>
+  <si>
+    <t>Implemented?</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -1527,11 +1533,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-936755056"/>
-        <c:axId val="-936753008"/>
+        <c:axId val="-1284966320"/>
+        <c:axId val="-1185793600"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-936755056"/>
+        <c:axId val="-1284966320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1574,14 +1580,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-936753008"/>
+        <c:crossAx val="-1185793600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-936753008"/>
+        <c:axId val="-1185793600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1632,7 +1638,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-936755056"/>
+        <c:crossAx val="-1284966320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2244,7 +2250,7 @@
         <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3230,7 +3236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -4223,8 +4229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4630,8 +4636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4828,11 +4834,11 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A21" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>63</v>
+      <c r="A21" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>293</v>
@@ -4847,11 +4853,11 @@
       <c r="I21" s="13"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A24" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>69</v>
+      <c r="A24" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>294</v>
@@ -4874,488 +4880,564 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:B22"/>
+    <sheetView topLeftCell="A8" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="251.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="251.83203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>42</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" t="s">
+        <v>316</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>34</v>
       </c>
       <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>32</v>
       </c>
       <c r="B6" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" t="s">
+        <v>316</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>48</v>
       </c>
       <c r="B7" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" t="s">
+        <v>316</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>54</v>
       </c>
       <c r="B8" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" t="s">
+        <v>316</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>50</v>
       </c>
       <c r="B9" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" t="s">
+        <v>316</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>56</v>
       </c>
       <c r="B10" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" t="s">
+        <v>316</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>70</v>
       </c>
       <c r="B11" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" t="s">
+        <v>316</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>107</v>
       </c>
       <c r="B12" t="s">
         <v>108</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" t="s">
+        <v>316</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>110</v>
       </c>
       <c r="B13" t="s">
         <v>111</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="D13" s="11" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>58</v>
       </c>
       <c r="B14" t="s">
         <v>283</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" t="s">
+        <v>316</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>114</v>
       </c>
       <c r="B15" t="s">
         <v>115</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="D15" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>117</v>
       </c>
       <c r="B16" t="s">
         <v>118</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="D16" s="11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>68</v>
       </c>
       <c r="B17" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="D17" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>62</v>
       </c>
       <c r="B18" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="D18" s="11" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>64</v>
       </c>
       <c r="B19" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" t="s">
+        <v>316</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>123</v>
       </c>
       <c r="B20" t="s">
         <v>124</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>126</v>
       </c>
       <c r="B21" t="s">
         <v>127</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="D21" s="11" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>129</v>
       </c>
       <c r="B22" t="s">
         <v>130</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" t="s">
+        <v>316</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>132</v>
       </c>
       <c r="B23" t="s">
         <v>133</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>135</v>
       </c>
       <c r="B24" t="s">
         <v>136</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="D24" s="11" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>138</v>
       </c>
       <c r="B25" t="s">
         <v>139</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="D25" s="11" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>141</v>
       </c>
       <c r="B26" t="s">
         <v>142</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="D26" s="11" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="32" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>30</v>
       </c>
       <c r="B27" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="D27" s="11" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>36</v>
       </c>
       <c r="B28" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" t="s">
+        <v>316</v>
+      </c>
+      <c r="D28" s="11" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>40</v>
       </c>
       <c r="B29" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" t="s">
+        <v>316</v>
+      </c>
+      <c r="D29" s="11" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>38</v>
       </c>
       <c r="B30" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" t="s">
+        <v>316</v>
+      </c>
+      <c r="D30" s="11" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>148</v>
       </c>
       <c r="B31" t="s">
         <v>149</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" t="s">
+        <v>316</v>
+      </c>
+      <c r="D31" s="11" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>52</v>
       </c>
       <c r="B32" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" t="s">
+        <v>316</v>
+      </c>
+      <c r="D32" s="11" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>152</v>
       </c>
       <c r="B33" t="s">
         <v>153</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="D33" s="11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>155</v>
       </c>
       <c r="B34" t="s">
         <v>156</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" t="s">
+        <v>316</v>
+      </c>
+      <c r="D34" s="11" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>158</v>
       </c>
       <c r="B35" t="s">
         <v>282</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" t="s">
+        <v>316</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>160</v>
       </c>
       <c r="B36" t="s">
         <v>161</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" t="s">
+        <v>316</v>
+      </c>
+      <c r="D36" s="11" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>163</v>
       </c>
       <c r="B37" t="s">
         <v>164</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" t="s">
+        <v>316</v>
+      </c>
+      <c r="D37" s="11" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>166</v>
       </c>
       <c r="B38" t="s">
         <v>167</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="D38" s="11" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>60</v>
       </c>
       <c r="B39" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="D39" s="11" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>66</v>
       </c>
       <c r="B40" t="s">
         <v>67</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="D40" s="11" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>24</v>
       </c>
       <c r="B41" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="D41" s="11" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>46</v>
       </c>
       <c r="B42" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" t="s">
+        <v>316</v>
+      </c>
+      <c r="D42" s="11" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>26</v>
       </c>
       <c r="B43" t="s">
         <v>27</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="D43" s="11" t="s">
         <v>173</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update with unittest cases for US21 and US33
</commit_message>
<xml_diff>
--- a/TeamGZWReport.xlsx
+++ b/TeamGZWReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" tabRatio="993" activeTab="6"/>
+    <workbookView xWindow="6400" yWindow="3240" windowWidth="25600" windowHeight="15560" tabRatio="993" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -4636,8 +4636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:B24"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4741,8 +4741,8 @@
       <c r="C10" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>290</v>
+      <c r="D10" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="E10" s="13">
         <v>60</v>
@@ -4750,8 +4750,12 @@
       <c r="F10" s="13">
         <v>100</v>
       </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
+      <c r="G10" s="13">
+        <v>23</v>
+      </c>
+      <c r="H10" s="13">
+        <v>30</v>
+      </c>
       <c r="I10" s="13"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
@@ -4796,8 +4800,8 @@
       <c r="C16" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="D16" s="13" t="s">
-        <v>290</v>
+      <c r="D16" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="E16" s="13">
         <v>40</v>
@@ -4805,8 +4809,12 @@
       <c r="F16" s="13">
         <v>50</v>
       </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
+      <c r="G16" s="13">
+        <v>10</v>
+      </c>
+      <c r="H16" s="13">
+        <v>30</v>
+      </c>
       <c r="I16" s="13"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update burndown chart and remove result image from previous submission
</commit_message>
<xml_diff>
--- a/TeamGZWReport.xlsx
+++ b/TeamGZWReport.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\SIT\SSW555\SSW555Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaojieli/Desktop/Spring2018/SSW555/Project/SSW555Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6405" yWindow="3240" windowWidth="25605" windowHeight="15555" tabRatio="993" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="21160" tabRatio="993" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Sprint4" sheetId="8" r:id="rId7"/>
     <sheet name="Stories" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1102,10 +1102,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="m/d"/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="m/d"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -1200,10 +1200,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1213,7 +1213,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1233,15 +1233,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1325,9 +1325,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1372,6 +1372,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1397,7 +1398,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1444,16 +1445,19 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41681</c:v>
+                  <c:v>41681.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41695</c:v>
+                  <c:v>41695.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41716</c:v>
+                  <c:v>41716.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41730</c:v>
+                  <c:v>41730.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41744.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1465,22 +1469,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-65F3-44CB-887C-3143EE86AB37}"/>
             </c:ext>
@@ -1523,16 +1530,19 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41681</c:v>
+                  <c:v>41681.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41695</c:v>
+                  <c:v>41695.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41716</c:v>
+                  <c:v>41716.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41730</c:v>
+                  <c:v>41730.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41744.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1544,22 +1554,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-65F3-44CB-887C-3143EE86AB37}"/>
             </c:ext>
@@ -1575,11 +1588,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1284966320"/>
-        <c:axId val="-1185793600"/>
+        <c:axId val="-1185513440"/>
+        <c:axId val="-1184761936"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-1284966320"/>
+        <c:axId val="-1185513440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1619,17 +1632,17 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1185793600"/>
+        <c:crossAx val="-1184761936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-1185793600"/>
+        <c:axId val="-1184761936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1677,10 +1690,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1284966320"/>
+        <c:crossAx val="-1185513440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1718,7 +1731,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2292,7 +2305,7 @@
         <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{13733394-7022-4B4B-B239-F4C10F9C3CB2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2582,13 +2595,13 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="27.625" customWidth="1"/>
-    <col min="5" max="5" width="25.125" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2605,7 +2618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2622,7 +2635,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2639,7 +2652,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2656,7 +2669,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="D9" s="1" t="s">
         <v>18</v>
       </c>
@@ -2688,12 +2701,12 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2713,7 +2726,7 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2734,7 +2747,7 @@
       <c r="AMI2"/>
       <c r="AMJ2"/>
     </row>
-    <row r="3" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2755,7 +2768,7 @@
       <c r="AMI3"/>
       <c r="AMJ3"/>
     </row>
-    <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2772,7 +2785,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2789,7 +2802,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2806,7 +2819,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2823,7 +2836,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2840,7 +2853,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2857,7 +2870,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2874,7 +2887,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="12" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2891,7 +2904,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="13" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2908,7 +2921,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="14" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2925,7 +2938,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="16" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1024" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>3</v>
       </c>
@@ -2939,7 +2952,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>3</v>
       </c>
@@ -2953,7 +2966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>3</v>
       </c>
@@ -2970,7 +2983,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2984,7 +2997,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2998,7 +3011,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>3</v>
       </c>
@@ -3015,7 +3028,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>4</v>
       </c>
@@ -3032,7 +3045,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>4</v>
       </c>
@@ -3049,7 +3062,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>4</v>
       </c>
@@ -3066,7 +3079,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>4</v>
       </c>
@@ -3083,7 +3096,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>4</v>
       </c>
@@ -3100,7 +3113,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>4</v>
       </c>
@@ -3129,21 +3142,21 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="26.375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.375" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="15.125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>72</v>
       </c>
@@ -3166,7 +3179,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>41681</v>
       </c>
@@ -3181,7 +3194,7 @@
       </c>
       <c r="G2"/>
     </row>
-    <row r="3" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>41695</v>
       </c>
@@ -3208,7 +3221,7 @@
         <v>32.857142857142861</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>41716</v>
       </c>
@@ -3234,7 +3247,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>41730</v>
       </c>
@@ -3260,10 +3273,33 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B6"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="3">
+        <v>41744</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <f>20+24+23+10</f>
+        <v>77</v>
+      </c>
+      <c r="F6">
+        <f>30+35+30+30</f>
+        <v>125</v>
+      </c>
+      <c r="G6" s="4">
+        <f>E6/F6*60</f>
+        <v>36.96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B7"/>
     </row>
   </sheetData>
@@ -3282,17 +3318,17 @@
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="26.125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="15.125" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="17.625" customWidth="1"/>
-    <col min="8" max="8" width="17.875" customWidth="1"/>
-    <col min="9" max="9" width="19.875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -3321,12 +3357,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="I2" s="5">
         <v>41695</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -3355,7 +3391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>80</v>
       </c>
@@ -3367,7 +3403,7 @@
       </c>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -3379,7 +3415,7 @@
       </c>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>84</v>
       </c>
@@ -3391,7 +3427,7 @@
       </c>
       <c r="I6"/>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -3420,7 +3456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -3432,7 +3468,7 @@
       </c>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>88</v>
       </c>
@@ -3444,7 +3480,7 @@
       </c>
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>90</v>
       </c>
@@ -3456,11 +3492,11 @@
       </c>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B11"/>
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -3486,7 +3522,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>173</v>
       </c>
@@ -3512,7 +3548,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>176</v>
       </c>
@@ -3538,7 +3574,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>178</v>
       </c>
@@ -3564,7 +3600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -3591,7 +3627,7 @@
       </c>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>180</v>
       </c>
@@ -3617,7 +3653,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>182</v>
       </c>
@@ -3643,7 +3679,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>184</v>
       </c>
@@ -3669,7 +3705,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
@@ -3696,7 +3732,7 @@
       </c>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>186</v>
       </c>
@@ -3704,7 +3740,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>188</v>
       </c>
@@ -3712,7 +3748,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
@@ -3739,7 +3775,7 @@
       </c>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>190</v>
       </c>
@@ -3747,7 +3783,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="39" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>192</v>
       </c>
@@ -3755,32 +3791,32 @@
         <v>193</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>235</v>
       </c>
@@ -3800,19 +3836,19 @@
       <selection activeCell="B29" sqref="B29:H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="32.5" customWidth="1"/>
-    <col min="3" max="3" width="11.125" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="17.125" customWidth="1"/>
-    <col min="6" max="6" width="21.125" customWidth="1"/>
-    <col min="7" max="7" width="16.125" customWidth="1"/>
-    <col min="8" max="8" width="21.125" customWidth="1"/>
-    <col min="9" max="9" width="17.125" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -3841,13 +3877,13 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B2" s="7"/>
       <c r="I2" s="5">
         <v>41716</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
         <v>40</v>
       </c>
@@ -3874,7 +3910,7 @@
       </c>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>205</v>
       </c>
@@ -3885,7 +3921,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>206</v>
       </c>
@@ -3896,7 +3932,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
@@ -3923,7 +3959,7 @@
       </c>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>209</v>
       </c>
@@ -3934,7 +3970,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>210</v>
       </c>
@@ -3945,7 +3981,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>269</v>
       </c>
@@ -3972,7 +4008,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>229</v>
       </c>
@@ -3984,7 +4020,7 @@
       </c>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>230</v>
       </c>
@@ -3996,11 +4032,11 @@
       </c>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B13" s="7"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -4027,7 +4063,7 @@
       </c>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>231</v>
       </c>
@@ -4039,7 +4075,7 @@
       </c>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>233</v>
       </c>
@@ -4051,11 +4087,11 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B17" s="7"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>50</v>
       </c>
@@ -4082,7 +4118,7 @@
       </c>
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>218</v>
       </c>
@@ -4091,7 +4127,7 @@
       </c>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>220</v>
       </c>
@@ -4100,7 +4136,7 @@
       </c>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>222</v>
       </c>
@@ -4109,11 +4145,11 @@
       </c>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B22" s="7"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>56</v>
       </c>
@@ -4140,7 +4176,7 @@
       </c>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>224</v>
       </c>
@@ -4149,7 +4185,7 @@
       </c>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>225</v>
       </c>
@@ -4158,7 +4194,7 @@
       </c>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>226</v>
       </c>
@@ -4166,7 +4202,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B29" s="15" t="s">
         <v>213</v>
       </c>
@@ -4178,7 +4214,7 @@
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B30" s="15" t="s">
         <v>238</v>
       </c>
@@ -4190,7 +4226,7 @@
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B31" s="15" t="s">
         <v>215</v>
       </c>
@@ -4202,7 +4238,7 @@
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B32" s="15" t="s">
         <v>216</v>
       </c>
@@ -4214,7 +4250,7 @@
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B33" s="15" t="s">
         <v>217</v>
       </c>
@@ -4226,7 +4262,7 @@
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B34" s="15"/>
       <c r="C34" s="16"/>
       <c r="D34" s="15"/>
@@ -4236,7 +4272,7 @@
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B35" s="15" t="s">
         <v>214</v>
       </c>
@@ -4248,7 +4284,7 @@
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B36" s="15" t="s">
         <v>239</v>
       </c>
@@ -4271,22 +4307,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B31" sqref="A26:B31"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="45.5" customWidth="1"/>
-    <col min="4" max="4" width="16.625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="18.375" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="23.125" customWidth="1"/>
-    <col min="9" max="9" width="19.625" customWidth="1"/>
+    <col min="8" max="8" width="23.1640625" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -4315,13 +4351,13 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B2" s="7"/>
       <c r="I2" s="5">
         <v>41730</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>156</v>
       </c>
@@ -4348,7 +4384,7 @@
       </c>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>265</v>
       </c>
@@ -4359,7 +4395,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>266</v>
       </c>
@@ -4370,7 +4406,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
         <v>58</v>
       </c>
@@ -4397,7 +4433,7 @@
       </c>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>278</v>
       </c>
@@ -4408,7 +4444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>279</v>
       </c>
@@ -4419,7 +4455,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>106</v>
       </c>
@@ -4445,7 +4481,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>246</v>
       </c>
@@ -4453,7 +4489,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>248</v>
       </c>
@@ -4461,7 +4497,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>250</v>
       </c>
@@ -4469,7 +4505,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>146</v>
       </c>
@@ -4495,7 +4531,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>252</v>
       </c>
@@ -4503,7 +4539,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>254</v>
       </c>
@@ -4511,7 +4547,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>158</v>
       </c>
@@ -4537,7 +4573,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>258</v>
       </c>
@@ -4549,7 +4585,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>260</v>
       </c>
@@ -4561,7 +4597,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>161</v>
       </c>
@@ -4587,7 +4623,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>262</v>
       </c>
@@ -4595,7 +4631,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>263</v>
       </c>
@@ -4603,7 +4639,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26" s="15" t="s">
         <v>213</v>
       </c>
@@ -4614,7 +4650,7 @@
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27" s="15" t="s">
         <v>309</v>
       </c>
@@ -4625,7 +4661,7 @@
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A28" s="15" t="s">
         <v>310</v>
       </c>
@@ -4636,7 +4672,7 @@
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A29" s="15"/>
       <c r="B29" s="16"/>
       <c r="C29" s="15"/>
@@ -4645,7 +4681,7 @@
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A30" s="15" t="s">
         <v>214</v>
       </c>
@@ -4656,7 +4692,7 @@
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A31" s="15" t="s">
         <v>311</v>
       </c>
@@ -4679,21 +4715,21 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="40.125" customWidth="1"/>
+    <col min="2" max="2" width="40.1640625" customWidth="1"/>
     <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="13.625" customWidth="1"/>
-    <col min="6" max="6" width="15.125" customWidth="1"/>
-    <col min="7" max="7" width="13.625" customWidth="1"/>
-    <col min="8" max="8" width="13.125" customWidth="1"/>
-    <col min="9" max="9" width="15.125" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -4722,12 +4758,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="I2" s="19">
         <v>41744</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
         <v>64</v>
       </c>
@@ -4754,7 +4790,7 @@
       </c>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>319</v>
       </c>
@@ -4762,7 +4798,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>320</v>
       </c>
@@ -4770,7 +4806,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
         <v>70</v>
       </c>
@@ -4797,7 +4833,7 @@
       </c>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>323</v>
       </c>
@@ -4805,7 +4841,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>325</v>
       </c>
@@ -4813,7 +4849,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>153</v>
       </c>
@@ -4840,7 +4876,7 @@
       </c>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>295</v>
       </c>
@@ -4848,7 +4884,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>297</v>
       </c>
@@ -4856,7 +4892,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>299</v>
       </c>
@@ -4864,7 +4900,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>301</v>
       </c>
@@ -4872,7 +4908,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>127</v>
       </c>
@@ -4899,7 +4935,7 @@
       </c>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>303</v>
       </c>
@@ -4907,7 +4943,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>305</v>
       </c>
@@ -4915,7 +4951,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>307</v>
       </c>
@@ -4923,7 +4959,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>109</v>
       </c>
@@ -4942,7 +4978,7 @@
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>133</v>
       </c>
@@ -4961,35 +4997,35 @@
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="15" t="s">
         <v>213</v>
       </c>
       <c r="B27" s="16"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="15" t="s">
         <v>309</v>
       </c>
       <c r="B28" s="16"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="15" t="s">
         <v>310</v>
       </c>
       <c r="B29" s="16"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="15"/>
       <c r="B30" s="16"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="15" t="s">
         <v>214</v>
       </c>
       <c r="B31" s="16"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="15" t="s">
         <v>318</v>
       </c>
@@ -5010,14 +5046,14 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="4" width="251.875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="251.83203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -5031,7 +5067,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -5045,7 +5081,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -5059,7 +5095,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -5073,7 +5109,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -5087,7 +5123,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -5101,7 +5137,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -5115,7 +5151,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -5129,7 +5165,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -5143,7 +5179,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -5157,7 +5193,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -5171,7 +5207,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>106</v>
       </c>
@@ -5185,7 +5221,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -5196,7 +5232,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -5210,7 +5246,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>113</v>
       </c>
@@ -5221,7 +5257,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>115</v>
       </c>
@@ -5232,7 +5268,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -5243,7 +5279,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -5254,7 +5290,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -5268,7 +5304,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>121</v>
       </c>
@@ -5279,7 +5315,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>124</v>
       </c>
@@ -5290,7 +5326,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -5304,7 +5340,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>130</v>
       </c>
@@ -5315,7 +5351,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>133</v>
       </c>
@@ -5326,7 +5362,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>136</v>
       </c>
@@ -5337,7 +5373,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>139</v>
       </c>
@@ -5348,7 +5384,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -5359,7 +5395,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -5373,7 +5409,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -5387,7 +5423,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -5401,7 +5437,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>146</v>
       </c>
@@ -5415,7 +5451,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -5429,7 +5465,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>150</v>
       </c>
@@ -5440,7 +5476,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>153</v>
       </c>
@@ -5454,7 +5490,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>156</v>
       </c>
@@ -5468,7 +5504,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>158</v>
       </c>
@@ -5482,7 +5518,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>161</v>
       </c>
@@ -5496,7 +5532,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>164</v>
       </c>
@@ -5507,7 +5543,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -5518,7 +5554,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>66</v>
       </c>
@@ -5529,7 +5565,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -5540,7 +5576,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -5554,7 +5590,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>26</v>
       </c>

</xml_diff>